<commit_message>
Added most of Run2 embryo data
</commit_message>
<xml_diff>
--- a/Ionocyte/All embryo ionocyte data.xlsx
+++ b/Ionocyte/All embryo ionocyte data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teres\Documents\GitHub\MenidiaOA\Ionocyte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A31C78-2B96-4544-99C6-293EA7CADFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0301FAE-D1F5-4B11-9B8E-8FA307AC7189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DAFCA9E7-78AB-4FDC-8B4B-32C2729B4956}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="111">
   <si>
     <t>Experiment</t>
   </si>
@@ -242,13 +242,139 @@
   </si>
   <si>
     <t xml:space="preserve">Units are already µm^2, skip for conversion from pixels. </t>
+  </si>
+  <si>
+    <t>run2</t>
+  </si>
+  <si>
+    <t>2016-41</t>
+  </si>
+  <si>
+    <t>2016-42</t>
+  </si>
+  <si>
+    <t>2016-43</t>
+  </si>
+  <si>
+    <t>2016-44</t>
+  </si>
+  <si>
+    <t>2016-45</t>
+  </si>
+  <si>
+    <t>2016-46</t>
+  </si>
+  <si>
+    <t>2016-47</t>
+  </si>
+  <si>
+    <t>2016-48</t>
+  </si>
+  <si>
+    <t>2016-49</t>
+  </si>
+  <si>
+    <t>2016-50</t>
+  </si>
+  <si>
+    <t>2016-51</t>
+  </si>
+  <si>
+    <t>2016-52</t>
+  </si>
+  <si>
+    <t>2016-53</t>
+  </si>
+  <si>
+    <t>2016-54</t>
+  </si>
+  <si>
+    <t>2016-55</t>
+  </si>
+  <si>
+    <t>2016-56</t>
+  </si>
+  <si>
+    <t>2016-57</t>
+  </si>
+  <si>
+    <t>2016-58</t>
+  </si>
+  <si>
+    <t>2016-59</t>
+  </si>
+  <si>
+    <t>2016-60</t>
+  </si>
+  <si>
+    <t>2016-61</t>
+  </si>
+  <si>
+    <t>2016-62</t>
+  </si>
+  <si>
+    <t>2016-63</t>
+  </si>
+  <si>
+    <t>2016-64</t>
+  </si>
+  <si>
+    <t>2016-65</t>
+  </si>
+  <si>
+    <t>2016-66</t>
+  </si>
+  <si>
+    <t>2016-67</t>
+  </si>
+  <si>
+    <t>2016-68</t>
+  </si>
+  <si>
+    <t>2016-69</t>
+  </si>
+  <si>
+    <t>2016-70</t>
+  </si>
+  <si>
+    <t>2016-71</t>
+  </si>
+  <si>
+    <t>2016-72</t>
+  </si>
+  <si>
+    <t>2016-73</t>
+  </si>
+  <si>
+    <t>2016-74</t>
+  </si>
+  <si>
+    <t>2016-75</t>
+  </si>
+  <si>
+    <t>2016-76</t>
+  </si>
+  <si>
+    <t>2016-77</t>
+  </si>
+  <si>
+    <t>2016-78</t>
+  </si>
+  <si>
+    <t>2016-79</t>
+  </si>
+  <si>
+    <t>2016-80</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,6 +384,20 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -289,12 +429,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,10 +750,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F1C880-24DC-4CF8-8C86-70B462FC0B54}">
-  <dimension ref="A1:X41"/>
+  <dimension ref="A1:X81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -621,77 +763,77 @@
     <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2455,7 +2597,1612 @@
         <v>129</v>
       </c>
     </row>
+    <row r="42" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="3">
+        <v>2016</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="O42" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="P42" s="3">
+        <v>275409.7</v>
+      </c>
+      <c r="Q42" s="3">
+        <v>6</v>
+      </c>
+      <c r="R42" s="3">
+        <v>512888.3</v>
+      </c>
+      <c r="S42" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="3">
+        <v>2016</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="O43" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="P43" s="3">
+        <v>225559.1</v>
+      </c>
+      <c r="Q43" s="3">
+        <v>45</v>
+      </c>
+      <c r="R43" s="3">
+        <v>720992</v>
+      </c>
+      <c r="S43" s="3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" s="3">
+        <v>2016</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="O44" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="P44" s="3">
+        <v>273320.2</v>
+      </c>
+      <c r="Q44" s="3">
+        <v>14</v>
+      </c>
+      <c r="R44" s="3">
+        <v>548776.19999999995</v>
+      </c>
+      <c r="S44" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P45" s="1">
+        <v>89594</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>12</v>
+      </c>
+      <c r="R45" s="1">
+        <v>105979</v>
+      </c>
+      <c r="S45" s="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="R46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="S46" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P47" s="1">
+        <v>45172</v>
+      </c>
+      <c r="Q47" s="1">
+        <v>9</v>
+      </c>
+      <c r="R47" s="1">
+        <v>141556</v>
+      </c>
+      <c r="S47" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="R48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="S48" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P49" s="1">
+        <v>63288</v>
+      </c>
+      <c r="Q49" s="1">
+        <v>21</v>
+      </c>
+      <c r="R49" s="1">
+        <v>96934</v>
+      </c>
+      <c r="S49" s="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O50" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P50" s="1">
+        <v>65111</v>
+      </c>
+      <c r="Q50" s="1">
+        <v>10</v>
+      </c>
+      <c r="R50" s="1">
+        <v>105485</v>
+      </c>
+      <c r="S50" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O51" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P51" s="1">
+        <v>58728</v>
+      </c>
+      <c r="Q51" s="1">
+        <v>4</v>
+      </c>
+      <c r="R51" s="1">
+        <v>108275</v>
+      </c>
+      <c r="S51" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O52" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P52" s="1">
+        <v>79167</v>
+      </c>
+      <c r="Q52" s="1">
+        <v>101</v>
+      </c>
+      <c r="R52" s="1">
+        <v>132460</v>
+      </c>
+      <c r="S52" s="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B53" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O53" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P53" s="1">
+        <v>43111</v>
+      </c>
+      <c r="Q53" s="1">
+        <v>43</v>
+      </c>
+      <c r="R53" s="1">
+        <v>166679</v>
+      </c>
+      <c r="S53" s="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B54" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O54" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P54" s="1">
+        <v>51710</v>
+      </c>
+      <c r="Q54" s="1">
+        <v>30</v>
+      </c>
+      <c r="R54" s="1">
+        <v>145267</v>
+      </c>
+      <c r="S54" s="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B55" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O55" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P55" s="1">
+        <v>75120</v>
+      </c>
+      <c r="Q55" s="1">
+        <v>18</v>
+      </c>
+      <c r="R55" s="1">
+        <v>116811</v>
+      </c>
+      <c r="S55" s="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B56" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P56" s="1">
+        <v>55340</v>
+      </c>
+      <c r="Q56" s="1">
+        <v>49</v>
+      </c>
+      <c r="R56" s="1">
+        <v>148063</v>
+      </c>
+      <c r="S56" s="1">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B57" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F57" s="1">
+        <v>396773</v>
+      </c>
+      <c r="G57" s="1">
+        <v>4</v>
+      </c>
+      <c r="H57" s="1">
+        <v>714993</v>
+      </c>
+      <c r="I57" s="1">
+        <v>62</v>
+      </c>
+      <c r="O57" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P57" s="1">
+        <v>418035</v>
+      </c>
+      <c r="Q57" s="1">
+        <v>79</v>
+      </c>
+      <c r="R57" s="1">
+        <v>546144</v>
+      </c>
+      <c r="S57" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B58" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F58" s="1">
+        <v>455533</v>
+      </c>
+      <c r="G58" s="1">
+        <v>38</v>
+      </c>
+      <c r="H58" s="1">
+        <v>582272</v>
+      </c>
+      <c r="I58" s="1">
+        <v>131</v>
+      </c>
+      <c r="O58" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P58" s="1">
+        <v>482208</v>
+      </c>
+      <c r="Q58" s="1">
+        <v>27</v>
+      </c>
+      <c r="R58" s="1">
+        <v>557279</v>
+      </c>
+      <c r="S58" s="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B59" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F59" s="1">
+        <v>354606</v>
+      </c>
+      <c r="G59" s="1">
+        <v>10</v>
+      </c>
+      <c r="H59" s="1">
+        <v>686786</v>
+      </c>
+      <c r="I59" s="1">
+        <v>183</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P59" s="1">
+        <v>436565</v>
+      </c>
+      <c r="Q59" s="1">
+        <v>23</v>
+      </c>
+      <c r="R59" s="1">
+        <v>605036</v>
+      </c>
+      <c r="S59" s="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B60" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F60" s="1">
+        <v>282445</v>
+      </c>
+      <c r="G60" s="1">
+        <v>5</v>
+      </c>
+      <c r="H60" s="1">
+        <v>630664</v>
+      </c>
+      <c r="I60" s="1">
+        <v>35</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P60" s="1">
+        <v>312004</v>
+      </c>
+      <c r="Q60" s="1">
+        <v>15</v>
+      </c>
+      <c r="R60" s="1">
+        <v>595675</v>
+      </c>
+      <c r="S60" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B61" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F61" s="1">
+        <v>427141</v>
+      </c>
+      <c r="G61" s="1">
+        <v>14</v>
+      </c>
+      <c r="H61" s="1">
+        <v>591219</v>
+      </c>
+      <c r="I61" s="1">
+        <v>111</v>
+      </c>
+      <c r="O61" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P61" s="1">
+        <v>441383</v>
+      </c>
+      <c r="Q61" s="1">
+        <v>18</v>
+      </c>
+      <c r="R61" s="1">
+        <v>565900</v>
+      </c>
+      <c r="S61" s="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B62" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F62" s="1">
+        <v>397516</v>
+      </c>
+      <c r="G62" s="1">
+        <v>7</v>
+      </c>
+      <c r="H62" s="1">
+        <v>513181</v>
+      </c>
+      <c r="I62" s="1">
+        <v>42</v>
+      </c>
+      <c r="O62" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P62" s="1">
+        <v>416384</v>
+      </c>
+      <c r="Q62" s="1">
+        <v>9</v>
+      </c>
+      <c r="R62" s="1">
+        <v>487953</v>
+      </c>
+      <c r="S62" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F63" s="1">
+        <v>313645</v>
+      </c>
+      <c r="G63" s="1">
+        <v>6</v>
+      </c>
+      <c r="H63" s="1">
+        <v>649714</v>
+      </c>
+      <c r="I63" s="1">
+        <v>9</v>
+      </c>
+      <c r="O63" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P63" s="1">
+        <v>308452</v>
+      </c>
+      <c r="Q63" s="1">
+        <v>2</v>
+      </c>
+      <c r="R63" s="1">
+        <v>646582</v>
+      </c>
+      <c r="S63" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B64" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F64" s="1">
+        <v>283520</v>
+      </c>
+      <c r="G64" s="1">
+        <v>4</v>
+      </c>
+      <c r="H64" s="1">
+        <v>567745</v>
+      </c>
+      <c r="I64" s="1">
+        <v>8</v>
+      </c>
+      <c r="O64" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P64" s="1">
+        <v>271332</v>
+      </c>
+      <c r="Q64" s="1">
+        <v>5</v>
+      </c>
+      <c r="R64" s="1">
+        <v>652626</v>
+      </c>
+      <c r="S64" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B65" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F65" s="1">
+        <v>446538</v>
+      </c>
+      <c r="G65" s="1">
+        <v>14</v>
+      </c>
+      <c r="H65" s="1">
+        <v>605410</v>
+      </c>
+      <c r="I65" s="1">
+        <v>20</v>
+      </c>
+      <c r="O65" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P65" s="1">
+        <v>343517</v>
+      </c>
+      <c r="Q65" s="1">
+        <v>1</v>
+      </c>
+      <c r="R65" s="1">
+        <v>692097</v>
+      </c>
+      <c r="S65" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B66" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F66" s="1">
+        <v>395342</v>
+      </c>
+      <c r="G66" s="1">
+        <v>14</v>
+      </c>
+      <c r="H66" s="1">
+        <v>638368</v>
+      </c>
+      <c r="I66" s="1">
+        <v>170</v>
+      </c>
+      <c r="O66" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P66" s="1">
+        <v>385221</v>
+      </c>
+      <c r="Q66" s="1">
+        <v>11</v>
+      </c>
+      <c r="R66" s="1">
+        <v>640567</v>
+      </c>
+      <c r="S66" s="1">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B67" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F67" s="1">
+        <v>318686</v>
+      </c>
+      <c r="G67" s="1">
+        <v>6</v>
+      </c>
+      <c r="H67" s="1">
+        <v>664416</v>
+      </c>
+      <c r="I67" s="1">
+        <v>73</v>
+      </c>
+      <c r="O67" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P67" s="1">
+        <v>317486</v>
+      </c>
+      <c r="Q67" s="1">
+        <v>8</v>
+      </c>
+      <c r="R67" s="1">
+        <v>645714</v>
+      </c>
+      <c r="S67" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B68" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F68" s="1">
+        <v>422470</v>
+      </c>
+      <c r="G68" s="1">
+        <v>24</v>
+      </c>
+      <c r="H68" s="1">
+        <v>684548</v>
+      </c>
+      <c r="I68" s="1">
+        <v>43</v>
+      </c>
+      <c r="O68" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P68" s="1">
+        <v>430320</v>
+      </c>
+      <c r="Q68" s="1">
+        <v>29</v>
+      </c>
+      <c r="R68" s="1">
+        <v>668158</v>
+      </c>
+      <c r="S68" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B69" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F69" s="1">
+        <v>405282</v>
+      </c>
+      <c r="G69" s="1">
+        <v>9</v>
+      </c>
+      <c r="H69" s="1">
+        <v>1111779</v>
+      </c>
+      <c r="I69" s="1">
+        <v>34</v>
+      </c>
+      <c r="O69" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P69" s="1">
+        <v>401413</v>
+      </c>
+      <c r="Q69" s="1">
+        <v>25</v>
+      </c>
+      <c r="R69" s="1">
+        <v>612733</v>
+      </c>
+      <c r="S69" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B70" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F70" s="1">
+        <v>261553</v>
+      </c>
+      <c r="G70" s="1">
+        <v>93</v>
+      </c>
+      <c r="H70" s="1">
+        <v>799096</v>
+      </c>
+      <c r="I70" s="1">
+        <v>145</v>
+      </c>
+      <c r="O70" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P70" s="1">
+        <v>459038</v>
+      </c>
+      <c r="Q70" s="1">
+        <v>26</v>
+      </c>
+      <c r="R70" s="1">
+        <v>590636</v>
+      </c>
+      <c r="S70" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B71" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F71" s="1">
+        <v>450983</v>
+      </c>
+      <c r="G71" s="1">
+        <v>59</v>
+      </c>
+      <c r="H71" s="1">
+        <v>446137</v>
+      </c>
+      <c r="I71" s="1">
+        <v>69</v>
+      </c>
+      <c r="O71" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P71" s="1">
+        <v>328811</v>
+      </c>
+      <c r="Q71" s="1">
+        <v>46</v>
+      </c>
+      <c r="R71" s="1">
+        <v>568451</v>
+      </c>
+      <c r="S71" s="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B72" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F72" s="1">
+        <v>363546</v>
+      </c>
+      <c r="G72" s="1">
+        <v>3</v>
+      </c>
+      <c r="H72" s="1">
+        <v>465818</v>
+      </c>
+      <c r="I72" s="1">
+        <v>22</v>
+      </c>
+      <c r="O72" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P72" s="1">
+        <v>408992</v>
+      </c>
+      <c r="Q72" s="1">
+        <v>7</v>
+      </c>
+      <c r="R72" s="1">
+        <v>499058</v>
+      </c>
+      <c r="S72" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B73" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F73" s="1">
+        <v>202320</v>
+      </c>
+      <c r="G73" s="1">
+        <v>25</v>
+      </c>
+      <c r="H73" s="1">
+        <v>924273</v>
+      </c>
+      <c r="I73" s="1">
+        <v>110</v>
+      </c>
+      <c r="O73" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P73" s="1">
+        <v>230601</v>
+      </c>
+      <c r="Q73" s="1">
+        <v>41</v>
+      </c>
+      <c r="R73" s="1">
+        <v>875988</v>
+      </c>
+      <c r="S73" s="1">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B74" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F74" s="1">
+        <v>430426</v>
+      </c>
+      <c r="G74" s="1">
+        <v>17</v>
+      </c>
+      <c r="H74" s="1">
+        <v>640751</v>
+      </c>
+      <c r="I74" s="1">
+        <v>30</v>
+      </c>
+      <c r="O74" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P74" s="1">
+        <v>459038</v>
+      </c>
+      <c r="Q74" s="1">
+        <v>26</v>
+      </c>
+      <c r="R74" s="1">
+        <v>590636</v>
+      </c>
+      <c r="S74" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B75" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F75" s="1">
+        <v>271403</v>
+      </c>
+      <c r="G75" s="1">
+        <v>7</v>
+      </c>
+      <c r="H75" s="1">
+        <v>692203</v>
+      </c>
+      <c r="I75" s="1">
+        <v>36</v>
+      </c>
+      <c r="O75" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P75" s="1">
+        <v>328811</v>
+      </c>
+      <c r="Q75" s="1">
+        <v>46</v>
+      </c>
+      <c r="R75" s="1">
+        <v>568451</v>
+      </c>
+      <c r="S75" s="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B76" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F76" s="1">
+        <v>249242</v>
+      </c>
+      <c r="G76" s="1">
+        <v>76</v>
+      </c>
+      <c r="H76" s="1">
+        <v>1085144</v>
+      </c>
+      <c r="I76" s="1">
+        <v>175</v>
+      </c>
+      <c r="O76" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P76" s="1">
+        <v>350752</v>
+      </c>
+      <c r="Q76" s="1">
+        <v>19</v>
+      </c>
+      <c r="R76" s="1">
+        <v>637831</v>
+      </c>
+      <c r="S76" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B77" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F77" s="1">
+        <v>414704</v>
+      </c>
+      <c r="G77" s="1">
+        <v>9</v>
+      </c>
+      <c r="H77" s="1">
+        <v>546033</v>
+      </c>
+      <c r="I77" s="1">
+        <v>80</v>
+      </c>
+      <c r="O77" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P77" s="1">
+        <v>438787</v>
+      </c>
+      <c r="Q77" s="1">
+        <v>23</v>
+      </c>
+      <c r="R77" s="1">
+        <v>553864</v>
+      </c>
+      <c r="S77" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B78" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F78" s="1">
+        <v>194074</v>
+      </c>
+      <c r="G78" s="1">
+        <v>6</v>
+      </c>
+      <c r="H78" s="1">
+        <v>630050</v>
+      </c>
+      <c r="I78" s="1">
+        <v>36</v>
+      </c>
+      <c r="O78" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P78" s="1">
+        <v>213866</v>
+      </c>
+      <c r="Q78" s="1">
+        <v>8</v>
+      </c>
+      <c r="R78" s="1">
+        <v>694596</v>
+      </c>
+      <c r="S78" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B79" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F79" s="1">
+        <v>256004</v>
+      </c>
+      <c r="G79" s="1">
+        <v>1</v>
+      </c>
+      <c r="H79" s="1">
+        <v>506890</v>
+      </c>
+      <c r="I79" s="1">
+        <v>12</v>
+      </c>
+      <c r="O79" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P79" s="1">
+        <v>327636</v>
+      </c>
+      <c r="Q79" s="1">
+        <v>6</v>
+      </c>
+      <c r="R79" s="1">
+        <v>454009</v>
+      </c>
+      <c r="S79" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B80" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O80" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="P80" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q80" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="R80" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="S80" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B81" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F81" s="1">
+        <v>484931</v>
+      </c>
+      <c r="G81" s="1">
+        <v>9</v>
+      </c>
+      <c r="H81" s="1">
+        <v>628406</v>
+      </c>
+      <c r="I81" s="1">
+        <v>41</v>
+      </c>
+      <c r="O81" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P81" s="1">
+        <v>519865</v>
+      </c>
+      <c r="Q81" s="1">
+        <v>19</v>
+      </c>
+      <c r="R81" s="1">
+        <v>729844</v>
+      </c>
+      <c r="S81" s="1">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Run 5 to data sheet
</commit_message>
<xml_diff>
--- a/Ionocyte/All embryo ionocyte data.xlsx
+++ b/Ionocyte/All embryo ionocyte data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teres\Documents\GitHub\MenidiaOA\Ionocyte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0301FAE-D1F5-4B11-9B8E-8FA307AC7189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E90791-92E4-4CE8-B1D1-E996FCE3D1A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DAFCA9E7-78AB-4FDC-8B4B-32C2729B4956}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="152">
   <si>
     <t>Experiment</t>
   </si>
@@ -368,6 +368,129 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>run5</t>
+  </si>
+  <si>
+    <t>2016-161</t>
+  </si>
+  <si>
+    <t>2016-162</t>
+  </si>
+  <si>
+    <t>2016-163</t>
+  </si>
+  <si>
+    <t>2016-164</t>
+  </si>
+  <si>
+    <t>2016-165</t>
+  </si>
+  <si>
+    <t>2016-166</t>
+  </si>
+  <si>
+    <t>2016-167</t>
+  </si>
+  <si>
+    <t>2016-168</t>
+  </si>
+  <si>
+    <t>2016-169</t>
+  </si>
+  <si>
+    <t>2016-170</t>
+  </si>
+  <si>
+    <t>2016-171</t>
+  </si>
+  <si>
+    <t>2016-172</t>
+  </si>
+  <si>
+    <t>2016-173</t>
+  </si>
+  <si>
+    <t>2016-174</t>
+  </si>
+  <si>
+    <t>2016-175</t>
+  </si>
+  <si>
+    <t>2016-176</t>
+  </si>
+  <si>
+    <t>2016-177</t>
+  </si>
+  <si>
+    <t>2016-178</t>
+  </si>
+  <si>
+    <t>2016-179</t>
+  </si>
+  <si>
+    <t>2016-180</t>
+  </si>
+  <si>
+    <t>2016-181</t>
+  </si>
+  <si>
+    <t>2016-182</t>
+  </si>
+  <si>
+    <t>2016-183</t>
+  </si>
+  <si>
+    <t>2016-184</t>
+  </si>
+  <si>
+    <t>2016-185</t>
+  </si>
+  <si>
+    <t>2016-186</t>
+  </si>
+  <si>
+    <t>2016-187</t>
+  </si>
+  <si>
+    <t>2016-188</t>
+  </si>
+  <si>
+    <t>2016-189</t>
+  </si>
+  <si>
+    <t>2016-190</t>
+  </si>
+  <si>
+    <t>2016-191</t>
+  </si>
+  <si>
+    <t>2016-192</t>
+  </si>
+  <si>
+    <t>2016-193</t>
+  </si>
+  <si>
+    <t>2016-194</t>
+  </si>
+  <si>
+    <t>2016-195</t>
+  </si>
+  <si>
+    <t>2016-196</t>
+  </si>
+  <si>
+    <t>2016-197</t>
+  </si>
+  <si>
+    <t>2016-198</t>
+  </si>
+  <si>
+    <t>2016-199</t>
+  </si>
+  <si>
+    <t>2016-200</t>
   </si>
 </sst>
 </file>
@@ -750,11 +873,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F1C880-24DC-4CF8-8C86-70B462FC0B54}">
-  <dimension ref="A1:X81"/>
+  <dimension ref="A1:X121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F53" sqref="F53"/>
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F95" sqref="F95:I95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2613,6 +2736,18 @@
       <c r="E42" s="3" t="s">
         <v>67</v>
       </c>
+      <c r="F42" s="3">
+        <v>281015.59999999998</v>
+      </c>
+      <c r="G42" s="3">
+        <v>4</v>
+      </c>
+      <c r="H42" s="3">
+        <v>501605.70000000007</v>
+      </c>
+      <c r="I42" s="3">
+        <v>6</v>
+      </c>
       <c r="O42" s="3" t="s">
         <v>67</v>
       </c>
@@ -2645,6 +2780,18 @@
       <c r="E43" s="3" t="s">
         <v>67</v>
       </c>
+      <c r="F43" s="3">
+        <v>213763.7</v>
+      </c>
+      <c r="G43" s="3">
+        <v>31</v>
+      </c>
+      <c r="H43" s="3">
+        <v>736598.29999999993</v>
+      </c>
+      <c r="I43" s="3">
+        <v>86</v>
+      </c>
       <c r="O43" s="3" t="s">
         <v>67</v>
       </c>
@@ -2677,6 +2824,18 @@
       <c r="E44" s="3" t="s">
         <v>67</v>
       </c>
+      <c r="F44" s="3">
+        <v>255275.4</v>
+      </c>
+      <c r="G44" s="3">
+        <v>13</v>
+      </c>
+      <c r="H44" s="3">
+        <v>562807.89999999991</v>
+      </c>
+      <c r="I44" s="3">
+        <v>26</v>
+      </c>
       <c r="O44" s="3" t="s">
         <v>67</v>
       </c>
@@ -2709,6 +2868,18 @@
       <c r="E45" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="F45" s="1">
+        <v>88296</v>
+      </c>
+      <c r="G45" s="1">
+        <v>10</v>
+      </c>
+      <c r="H45" s="1">
+        <v>105380</v>
+      </c>
+      <c r="I45" s="1">
+        <v>47</v>
+      </c>
       <c r="O45" s="1" t="s">
         <v>67</v>
       </c>
@@ -2785,6 +2956,18 @@
       <c r="E47" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F47" s="1">
+        <v>43415</v>
+      </c>
+      <c r="G47" s="1">
+        <v>6</v>
+      </c>
+      <c r="H47" s="1">
+        <v>135724</v>
+      </c>
+      <c r="I47" s="1">
+        <v>10</v>
+      </c>
       <c r="O47" s="1" t="s">
         <v>66</v>
       </c>
@@ -2861,6 +3044,18 @@
       <c r="E49" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F49" s="1">
+        <v>52390</v>
+      </c>
+      <c r="G49" s="1">
+        <v>14</v>
+      </c>
+      <c r="H49" s="1">
+        <v>101734</v>
+      </c>
+      <c r="I49" s="1">
+        <v>83</v>
+      </c>
       <c r="O49" s="1" t="s">
         <v>66</v>
       </c>
@@ -2893,6 +3088,18 @@
       <c r="E50" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F50" s="1">
+        <v>64399</v>
+      </c>
+      <c r="G50" s="1">
+        <v>16</v>
+      </c>
+      <c r="H50" s="1">
+        <v>111679</v>
+      </c>
+      <c r="I50" s="1">
+        <v>25</v>
+      </c>
       <c r="O50" s="1" t="s">
         <v>66</v>
       </c>
@@ -2925,6 +3132,18 @@
       <c r="E51" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="F51" s="1">
+        <v>60539</v>
+      </c>
+      <c r="G51" s="1">
+        <v>2</v>
+      </c>
+      <c r="H51" s="1">
+        <v>107661</v>
+      </c>
+      <c r="I51" s="1">
+        <v>8</v>
+      </c>
       <c r="O51" s="1" t="s">
         <v>67</v>
       </c>
@@ -2957,6 +3176,18 @@
       <c r="E52" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F52" s="1">
+        <v>78584</v>
+      </c>
+      <c r="G52" s="1">
+        <v>95</v>
+      </c>
+      <c r="H52" s="1">
+        <v>141277</v>
+      </c>
+      <c r="I52" s="1">
+        <v>124</v>
+      </c>
       <c r="O52" s="1" t="s">
         <v>66</v>
       </c>
@@ -2989,6 +3220,18 @@
       <c r="E53" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="F53" s="1">
+        <v>37602</v>
+      </c>
+      <c r="G53" s="1">
+        <v>28</v>
+      </c>
+      <c r="H53" s="1">
+        <v>180666</v>
+      </c>
+      <c r="I53" s="1">
+        <v>87</v>
+      </c>
       <c r="O53" s="1" t="s">
         <v>67</v>
       </c>
@@ -3021,6 +3264,18 @@
       <c r="E54" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="F54" s="1">
+        <v>46140</v>
+      </c>
+      <c r="G54" s="1">
+        <v>21</v>
+      </c>
+      <c r="H54" s="1">
+        <v>143964</v>
+      </c>
+      <c r="I54" s="1">
+        <v>81</v>
+      </c>
       <c r="O54" s="1" t="s">
         <v>67</v>
       </c>
@@ -3053,6 +3308,18 @@
       <c r="E55" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="F55" s="1">
+        <v>75842</v>
+      </c>
+      <c r="G55" s="1">
+        <v>10</v>
+      </c>
+      <c r="H55" s="1">
+        <v>113078</v>
+      </c>
+      <c r="I55" s="1">
+        <v>118</v>
+      </c>
       <c r="O55" s="1" t="s">
         <v>67</v>
       </c>
@@ -3085,6 +3352,18 @@
       <c r="E56" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="F56" s="1">
+        <v>50086</v>
+      </c>
+      <c r="G56" s="1">
+        <v>34</v>
+      </c>
+      <c r="H56" s="1">
+        <v>143173</v>
+      </c>
+      <c r="I56" s="1">
+        <v>116</v>
+      </c>
       <c r="O56" s="1" t="s">
         <v>67</v>
       </c>
@@ -4199,6 +4478,1766 @@
       </c>
       <c r="S81" s="1">
         <v>39</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B82" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F82" s="1">
+        <v>290447</v>
+      </c>
+      <c r="G82" s="1">
+        <v>38</v>
+      </c>
+      <c r="H82" s="1">
+        <v>484826</v>
+      </c>
+      <c r="I82" s="1">
+        <v>107</v>
+      </c>
+      <c r="O82" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P82" s="1">
+        <v>298690</v>
+      </c>
+      <c r="Q82" s="1">
+        <v>27</v>
+      </c>
+      <c r="R82" s="1">
+        <v>632542</v>
+      </c>
+      <c r="S82" s="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B83" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F83" s="1">
+        <v>220884</v>
+      </c>
+      <c r="G83" s="1">
+        <v>20</v>
+      </c>
+      <c r="H83" s="1">
+        <v>688483</v>
+      </c>
+      <c r="I83" s="1">
+        <v>44</v>
+      </c>
+      <c r="O83" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P83" s="1">
+        <v>229022</v>
+      </c>
+      <c r="Q83" s="1">
+        <v>34</v>
+      </c>
+      <c r="R83" s="1">
+        <v>647740</v>
+      </c>
+      <c r="S83" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B84" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F84" s="1">
+        <v>208526</v>
+      </c>
+      <c r="G84" s="1">
+        <v>10</v>
+      </c>
+      <c r="H84" s="1">
+        <v>577470</v>
+      </c>
+      <c r="I84" s="1">
+        <v>7</v>
+      </c>
+      <c r="O84" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P84" s="1">
+        <v>202218</v>
+      </c>
+      <c r="Q84" s="1">
+        <v>10</v>
+      </c>
+      <c r="R84" s="1">
+        <v>574700</v>
+      </c>
+      <c r="S84" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B85" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F85" s="1">
+        <v>299212</v>
+      </c>
+      <c r="G85" s="1">
+        <v>43</v>
+      </c>
+      <c r="H85" s="1">
+        <v>645358</v>
+      </c>
+      <c r="I85" s="1">
+        <v>100</v>
+      </c>
+      <c r="O85" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P85" s="1">
+        <v>329155</v>
+      </c>
+      <c r="Q85" s="1">
+        <v>38</v>
+      </c>
+      <c r="R85" s="1">
+        <v>603368</v>
+      </c>
+      <c r="S85" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B86" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F86" s="1">
+        <v>295306</v>
+      </c>
+      <c r="G86" s="1">
+        <v>4</v>
+      </c>
+      <c r="H86" s="1">
+        <v>602827</v>
+      </c>
+      <c r="I86" s="1">
+        <v>55</v>
+      </c>
+      <c r="O86" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P86" s="1">
+        <v>299941</v>
+      </c>
+      <c r="Q86" s="1">
+        <v>8</v>
+      </c>
+      <c r="R86" s="1">
+        <v>611533</v>
+      </c>
+      <c r="S86" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B87" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F87" s="1">
+        <v>142697</v>
+      </c>
+      <c r="G87" s="1">
+        <v>19</v>
+      </c>
+      <c r="H87" s="1">
+        <v>693231</v>
+      </c>
+      <c r="I87" s="1">
+        <v>26</v>
+      </c>
+      <c r="O87" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P87" s="1">
+        <v>196876</v>
+      </c>
+      <c r="Q87" s="1">
+        <v>23</v>
+      </c>
+      <c r="R87" s="1">
+        <v>636760</v>
+      </c>
+      <c r="S87" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B88" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F88" s="1">
+        <v>333381</v>
+      </c>
+      <c r="G88" s="1">
+        <v>17</v>
+      </c>
+      <c r="H88" s="1">
+        <v>693837</v>
+      </c>
+      <c r="I88" s="1">
+        <v>104</v>
+      </c>
+      <c r="O88" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P88" s="1">
+        <v>306929</v>
+      </c>
+      <c r="Q88" s="1">
+        <v>22</v>
+      </c>
+      <c r="R88" s="1">
+        <v>752739</v>
+      </c>
+      <c r="S88" s="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B89" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F89" s="1">
+        <v>329880</v>
+      </c>
+      <c r="G89" s="1">
+        <v>0</v>
+      </c>
+      <c r="H89" s="1">
+        <v>659650</v>
+      </c>
+      <c r="I89" s="1">
+        <v>17</v>
+      </c>
+      <c r="O89" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P89" s="1">
+        <v>339127</v>
+      </c>
+      <c r="Q89" s="1">
+        <v>3</v>
+      </c>
+      <c r="R89" s="1">
+        <v>646971</v>
+      </c>
+      <c r="S89" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B90" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F90" s="1">
+        <v>199239</v>
+      </c>
+      <c r="G90" s="1">
+        <v>5</v>
+      </c>
+      <c r="H90" s="1">
+        <v>659176</v>
+      </c>
+      <c r="I90" s="1">
+        <v>33</v>
+      </c>
+      <c r="O90" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P90" s="1">
+        <v>257253</v>
+      </c>
+      <c r="Q90" s="1">
+        <v>36</v>
+      </c>
+      <c r="R90" s="1">
+        <v>653254</v>
+      </c>
+      <c r="S90" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B91" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F91" s="1">
+        <v>312561</v>
+      </c>
+      <c r="G91" s="1">
+        <v>13</v>
+      </c>
+      <c r="H91" s="1">
+        <v>621177</v>
+      </c>
+      <c r="I91" s="1">
+        <v>49</v>
+      </c>
+      <c r="O91" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P91" s="1">
+        <v>338025</v>
+      </c>
+      <c r="Q91" s="1">
+        <v>13</v>
+      </c>
+      <c r="R91" s="1">
+        <v>515015</v>
+      </c>
+      <c r="S91" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B92" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F92" s="1">
+        <v>367121</v>
+      </c>
+      <c r="G92" s="1">
+        <v>27</v>
+      </c>
+      <c r="H92" s="1">
+        <v>588912</v>
+      </c>
+      <c r="I92" s="1">
+        <v>81</v>
+      </c>
+      <c r="O92" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P92" s="1">
+        <v>239185</v>
+      </c>
+      <c r="Q92" s="1">
+        <v>31</v>
+      </c>
+      <c r="R92" s="1">
+        <v>603435</v>
+      </c>
+      <c r="S92" s="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B93" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F93" s="1">
+        <v>181867</v>
+      </c>
+      <c r="G93" s="1">
+        <v>20</v>
+      </c>
+      <c r="H93" s="1">
+        <v>754898</v>
+      </c>
+      <c r="I93" s="1">
+        <v>97</v>
+      </c>
+      <c r="O93" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P93" s="1">
+        <v>183313</v>
+      </c>
+      <c r="Q93" s="1">
+        <v>29</v>
+      </c>
+      <c r="R93" s="1">
+        <v>712784</v>
+      </c>
+      <c r="S93" s="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B94" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F94" s="1">
+        <v>198732</v>
+      </c>
+      <c r="G94" s="1">
+        <v>2</v>
+      </c>
+      <c r="H94" s="1">
+        <v>743890</v>
+      </c>
+      <c r="I94" s="1">
+        <v>33</v>
+      </c>
+      <c r="O94" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P94" s="1">
+        <v>230573</v>
+      </c>
+      <c r="Q94" s="1">
+        <v>8</v>
+      </c>
+      <c r="R94" s="1">
+        <v>695811</v>
+      </c>
+      <c r="S94" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B95" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O95" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="P95" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q95" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="R95" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="S95" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B96" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F96" s="1">
+        <v>324175</v>
+      </c>
+      <c r="G96" s="1">
+        <v>10</v>
+      </c>
+      <c r="H96" s="1">
+        <v>569214</v>
+      </c>
+      <c r="I96" s="1">
+        <v>74</v>
+      </c>
+      <c r="O96" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P96" s="1">
+        <v>335478</v>
+      </c>
+      <c r="Q96" s="1">
+        <v>17</v>
+      </c>
+      <c r="R96" s="1">
+        <v>568367</v>
+      </c>
+      <c r="S96" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B97" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F97" s="1">
+        <v>342599</v>
+      </c>
+      <c r="G97" s="1">
+        <v>18</v>
+      </c>
+      <c r="H97" s="1">
+        <v>492540</v>
+      </c>
+      <c r="I97" s="1">
+        <v>52</v>
+      </c>
+      <c r="O97" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P97" s="1">
+        <v>374181</v>
+      </c>
+      <c r="Q97" s="1">
+        <v>21</v>
+      </c>
+      <c r="R97" s="1">
+        <v>458104</v>
+      </c>
+      <c r="S97" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B98" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F98" s="1">
+        <v>289862</v>
+      </c>
+      <c r="G98" s="1">
+        <v>4</v>
+      </c>
+      <c r="H98" s="1">
+        <v>514635</v>
+      </c>
+      <c r="I98" s="1">
+        <v>22</v>
+      </c>
+      <c r="O98" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P98" s="1">
+        <v>343846</v>
+      </c>
+      <c r="Q98" s="1">
+        <v>16</v>
+      </c>
+      <c r="R98" s="1">
+        <v>460972</v>
+      </c>
+      <c r="S98" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B99" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O99" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="P99" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q99" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="R99" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="S99" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B100" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F100" s="1">
+        <v>354031</v>
+      </c>
+      <c r="G100" s="1">
+        <v>14</v>
+      </c>
+      <c r="H100" s="1">
+        <v>788177</v>
+      </c>
+      <c r="I100" s="1">
+        <v>107</v>
+      </c>
+      <c r="O100" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P100" s="1">
+        <v>353071</v>
+      </c>
+      <c r="Q100" s="1">
+        <v>27</v>
+      </c>
+      <c r="R100" s="1">
+        <v>759197</v>
+      </c>
+      <c r="S100" s="1">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B101" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F101" s="1">
+        <v>537387</v>
+      </c>
+      <c r="G101" s="1">
+        <v>28</v>
+      </c>
+      <c r="H101" s="1">
+        <v>536765</v>
+      </c>
+      <c r="I101" s="1">
+        <v>33</v>
+      </c>
+      <c r="O101" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P101" s="1">
+        <v>521772</v>
+      </c>
+      <c r="Q101" s="1">
+        <v>15</v>
+      </c>
+      <c r="R101" s="1">
+        <v>515679</v>
+      </c>
+      <c r="S101" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B102" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F102" s="1">
+        <v>328308</v>
+      </c>
+      <c r="G102" s="1">
+        <v>29</v>
+      </c>
+      <c r="H102" s="1">
+        <v>624285</v>
+      </c>
+      <c r="I102" s="1">
+        <v>79</v>
+      </c>
+      <c r="O102" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P102" s="1">
+        <v>307011</v>
+      </c>
+      <c r="Q102" s="1">
+        <v>34</v>
+      </c>
+      <c r="R102" s="1">
+        <v>630086</v>
+      </c>
+      <c r="S102" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B103" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F103" s="1">
+        <v>425649</v>
+      </c>
+      <c r="G103" s="1">
+        <v>14</v>
+      </c>
+      <c r="H103" s="1">
+        <v>545475</v>
+      </c>
+      <c r="I103" s="1">
+        <v>67</v>
+      </c>
+      <c r="O103" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P103" s="1">
+        <v>401003</v>
+      </c>
+      <c r="Q103" s="1">
+        <v>12</v>
+      </c>
+      <c r="R103" s="1">
+        <v>579791</v>
+      </c>
+      <c r="S103" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A104" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B104" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F104" s="1">
+        <v>559443</v>
+      </c>
+      <c r="G104" s="1">
+        <v>6</v>
+      </c>
+      <c r="H104" s="1">
+        <v>393715</v>
+      </c>
+      <c r="I104" s="1">
+        <v>58</v>
+      </c>
+      <c r="O104" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P104" s="1">
+        <v>572852</v>
+      </c>
+      <c r="Q104" s="1">
+        <v>12</v>
+      </c>
+      <c r="R104" s="1">
+        <v>402504</v>
+      </c>
+      <c r="S104" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B105" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F105" s="1">
+        <v>576439</v>
+      </c>
+      <c r="G105" s="1">
+        <v>18</v>
+      </c>
+      <c r="H105" s="1">
+        <v>393845</v>
+      </c>
+      <c r="I105" s="1">
+        <v>13</v>
+      </c>
+      <c r="O105" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P105" s="1">
+        <v>596071</v>
+      </c>
+      <c r="Q105" s="1">
+        <v>21</v>
+      </c>
+      <c r="R105" s="1">
+        <v>376076</v>
+      </c>
+      <c r="S105" s="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B106" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F106" s="1">
+        <v>456561</v>
+      </c>
+      <c r="G106" s="1">
+        <v>6</v>
+      </c>
+      <c r="H106" s="1">
+        <v>505561</v>
+      </c>
+      <c r="I106" s="1">
+        <v>77</v>
+      </c>
+      <c r="O106" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P106" s="1">
+        <v>482179</v>
+      </c>
+      <c r="Q106" s="1">
+        <v>2</v>
+      </c>
+      <c r="R106" s="1">
+        <v>483500</v>
+      </c>
+      <c r="S106" s="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B107" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O107" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="P107" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q107" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="R107" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="S107" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B108" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F108" s="1">
+        <v>342268</v>
+      </c>
+      <c r="G108" s="1">
+        <v>16</v>
+      </c>
+      <c r="H108" s="1">
+        <v>365228</v>
+      </c>
+      <c r="I108" s="1">
+        <v>54</v>
+      </c>
+      <c r="O108" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P108" s="1">
+        <v>348773</v>
+      </c>
+      <c r="Q108" s="1">
+        <v>9</v>
+      </c>
+      <c r="R108" s="1">
+        <v>388205</v>
+      </c>
+      <c r="S108" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B109" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F109" s="1">
+        <v>370879</v>
+      </c>
+      <c r="G109" s="1">
+        <v>13</v>
+      </c>
+      <c r="H109" s="1">
+        <v>481239</v>
+      </c>
+      <c r="I109" s="1">
+        <v>27</v>
+      </c>
+      <c r="O109" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P109" s="1">
+        <v>362002</v>
+      </c>
+      <c r="Q109" s="1">
+        <v>22</v>
+      </c>
+      <c r="R109" s="1">
+        <v>445441</v>
+      </c>
+      <c r="S109" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B110" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F110" s="1">
+        <v>288784</v>
+      </c>
+      <c r="G110" s="1">
+        <v>43</v>
+      </c>
+      <c r="H110" s="1">
+        <v>624801</v>
+      </c>
+      <c r="I110" s="1">
+        <v>91</v>
+      </c>
+      <c r="O110" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P110" s="1">
+        <v>281932</v>
+      </c>
+      <c r="Q110" s="1">
+        <v>28</v>
+      </c>
+      <c r="R110" s="1">
+        <v>668195</v>
+      </c>
+      <c r="S110" s="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B111" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F111" s="1">
+        <v>425825</v>
+      </c>
+      <c r="G111" s="1">
+        <v>8</v>
+      </c>
+      <c r="H111" s="1">
+        <v>583501</v>
+      </c>
+      <c r="I111" s="1">
+        <v>63</v>
+      </c>
+      <c r="O111" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P111" s="1">
+        <v>432617</v>
+      </c>
+      <c r="Q111" s="1">
+        <v>12</v>
+      </c>
+      <c r="R111" s="1">
+        <v>555459</v>
+      </c>
+      <c r="S111" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B112" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F112" s="1">
+        <v>189614</v>
+      </c>
+      <c r="G112" s="1">
+        <v>54</v>
+      </c>
+      <c r="H112" s="1">
+        <v>750319</v>
+      </c>
+      <c r="I112" s="1">
+        <v>120</v>
+      </c>
+      <c r="O112" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P112" s="1">
+        <v>165489</v>
+      </c>
+      <c r="Q112" s="1">
+        <v>99</v>
+      </c>
+      <c r="R112" s="1">
+        <v>712724</v>
+      </c>
+      <c r="S112" s="1">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B113" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O113" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="P113" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q113" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="R113" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="S113" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B114" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F114" s="1">
+        <v>223656</v>
+      </c>
+      <c r="G114" s="1">
+        <v>2</v>
+      </c>
+      <c r="H114" s="1">
+        <v>618596</v>
+      </c>
+      <c r="I114" s="1">
+        <v>14</v>
+      </c>
+      <c r="O114" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P114" s="1">
+        <v>228754</v>
+      </c>
+      <c r="Q114" s="1">
+        <v>0</v>
+      </c>
+      <c r="R114" s="1">
+        <v>641278</v>
+      </c>
+      <c r="S114" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B115" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F115" s="1">
+        <v>319151</v>
+      </c>
+      <c r="G115" s="1">
+        <v>18</v>
+      </c>
+      <c r="H115" s="1">
+        <v>623408</v>
+      </c>
+      <c r="I115" s="1">
+        <v>13</v>
+      </c>
+      <c r="O115" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P115" s="1">
+        <v>436718</v>
+      </c>
+      <c r="Q115" s="1">
+        <v>58</v>
+      </c>
+      <c r="R115" s="1">
+        <v>490818</v>
+      </c>
+      <c r="S115" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B116" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F116" s="1">
+        <v>292135</v>
+      </c>
+      <c r="G116" s="1">
+        <v>63</v>
+      </c>
+      <c r="H116" s="1">
+        <v>684058</v>
+      </c>
+      <c r="I116" s="1">
+        <v>103</v>
+      </c>
+      <c r="O116" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P116" s="1">
+        <v>291756</v>
+      </c>
+      <c r="Q116" s="1">
+        <v>63</v>
+      </c>
+      <c r="R116" s="1">
+        <v>686635</v>
+      </c>
+      <c r="S116" s="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B117" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F117" s="1">
+        <v>313585</v>
+      </c>
+      <c r="G117" s="1">
+        <v>24</v>
+      </c>
+      <c r="H117" s="1">
+        <v>785193</v>
+      </c>
+      <c r="I117" s="1">
+        <v>124</v>
+      </c>
+      <c r="O117" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P117" s="1">
+        <v>364682</v>
+      </c>
+      <c r="Q117" s="1">
+        <v>24</v>
+      </c>
+      <c r="R117" s="1">
+        <v>729254</v>
+      </c>
+      <c r="S117" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B118" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F118" s="1">
+        <v>372231</v>
+      </c>
+      <c r="G118" s="1">
+        <v>23</v>
+      </c>
+      <c r="H118" s="1">
+        <v>638051</v>
+      </c>
+      <c r="I118" s="1">
+        <v>118</v>
+      </c>
+      <c r="O118" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P118" s="1">
+        <v>422941</v>
+      </c>
+      <c r="Q118" s="1">
+        <v>36</v>
+      </c>
+      <c r="R118" s="1">
+        <v>575638</v>
+      </c>
+      <c r="S118" s="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B119" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I119" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O119" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="P119" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q119" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="R119" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="S119" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A120" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B120" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I120" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O120" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="P120" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q120" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="R120" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="S120" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A121" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B121" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F121" s="1">
+        <v>219703</v>
+      </c>
+      <c r="G121" s="1">
+        <v>24</v>
+      </c>
+      <c r="H121" s="1">
+        <v>814354</v>
+      </c>
+      <c r="I121" s="1">
+        <v>233</v>
+      </c>
+      <c r="O121" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P121" s="1">
+        <v>330236</v>
+      </c>
+      <c r="Q121" s="1">
+        <v>16</v>
+      </c>
+      <c r="R121" s="1">
+        <v>668678</v>
+      </c>
+      <c r="S121" s="1">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited color highlighting of embryo ionocyte data sheet
</commit_message>
<xml_diff>
--- a/Ionocyte/All embryo ionocyte data.xlsx
+++ b/Ionocyte/All embryo ionocyte data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teres\Documents\GitHub\MenidiaOA\Ionocyte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E90791-92E4-4CE8-B1D1-E996FCE3D1A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BECC014-9EB4-453D-856A-7509769C1B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DAFCA9E7-78AB-4FDC-8B4B-32C2729B4956}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="153">
   <si>
     <t>Experiment</t>
   </si>
@@ -241,9 +241,6 @@
     <t>L</t>
   </si>
   <si>
-    <t xml:space="preserve">Units are already µm^2, skip for conversion from pixels. </t>
-  </si>
-  <si>
     <t>run2</t>
   </si>
   <si>
@@ -491,6 +488,12 @@
   </si>
   <si>
     <t>2016-200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used Frisk lab microscope. Units are already µm^2, skip for conversion from pixels. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used dissecting microscope. Pixel sizes are different from the other samples. </t>
   </si>
 </sst>
 </file>
@@ -526,7 +529,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -536,6 +539,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -552,13 +561,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -876,8 +887,8 @@
   <dimension ref="A1:X121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F95" sqref="F95:I95"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2728,10 +2739,10 @@
         <v>2016</v>
       </c>
       <c r="C42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>67</v>
@@ -2772,10 +2783,10 @@
         <v>2016</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>67</v>
@@ -2816,10 +2827,10 @@
         <v>2016</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>67</v>
@@ -2852,531 +2863,531 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B45" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D45" s="1" t="s">
+    <row r="45" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" s="6">
+        <v>2016</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F45" s="6">
+        <v>88296</v>
+      </c>
+      <c r="G45" s="6">
+        <v>10</v>
+      </c>
+      <c r="H45" s="6">
+        <v>105380</v>
+      </c>
+      <c r="I45" s="6">
+        <v>47</v>
+      </c>
+      <c r="O45" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="P45" s="6">
+        <v>89594</v>
+      </c>
+      <c r="Q45" s="6">
+        <v>12</v>
+      </c>
+      <c r="R45" s="6">
+        <v>105979</v>
+      </c>
+      <c r="S45" s="6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" s="6">
+        <v>2016</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D46" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F45" s="1">
-        <v>88296</v>
-      </c>
-      <c r="G45" s="1">
+      <c r="E46" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="O46" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="P46" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q46" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="R46" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="S46" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="6">
+        <v>2016</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F47" s="6">
+        <v>43415</v>
+      </c>
+      <c r="G47" s="6">
+        <v>6</v>
+      </c>
+      <c r="H47" s="6">
+        <v>135724</v>
+      </c>
+      <c r="I47" s="6">
         <v>10</v>
       </c>
-      <c r="H45" s="1">
-        <v>105380</v>
-      </c>
-      <c r="I45" s="1">
-        <v>47</v>
-      </c>
-      <c r="O45" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="P45" s="1">
-        <v>89594</v>
-      </c>
-      <c r="Q45" s="1">
-        <v>12</v>
-      </c>
-      <c r="R45" s="1">
-        <v>105979</v>
-      </c>
-      <c r="S45" s="1">
+      <c r="O47" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="P47" s="6">
+        <v>45172</v>
+      </c>
+      <c r="Q47" s="6">
+        <v>9</v>
+      </c>
+      <c r="R47" s="6">
+        <v>141556</v>
+      </c>
+      <c r="S47" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" s="6">
+        <v>2016</v>
+      </c>
+      <c r="C48" s="6" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B46" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="O46" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="P46" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q46" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="R46" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="S46" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B47" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D47" s="1" t="s">
+      <c r="D48" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F47" s="1">
-        <v>43415</v>
-      </c>
-      <c r="G47" s="1">
-        <v>6</v>
-      </c>
-      <c r="H47" s="1">
-        <v>135724</v>
-      </c>
-      <c r="I47" s="1">
+      <c r="E48" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="O48" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="P48" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q48" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="R48" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="S48" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" s="6">
+        <v>2016</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F49" s="6">
+        <v>52390</v>
+      </c>
+      <c r="G49" s="6">
+        <v>14</v>
+      </c>
+      <c r="H49" s="6">
+        <v>101734</v>
+      </c>
+      <c r="I49" s="6">
+        <v>83</v>
+      </c>
+      <c r="O49" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="P49" s="6">
+        <v>63288</v>
+      </c>
+      <c r="Q49" s="6">
+        <v>21</v>
+      </c>
+      <c r="R49" s="6">
+        <v>96934</v>
+      </c>
+      <c r="S49" s="6">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" s="6">
+        <v>2016</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F50" s="6">
+        <v>64399</v>
+      </c>
+      <c r="G50" s="6">
+        <v>16</v>
+      </c>
+      <c r="H50" s="6">
+        <v>111679</v>
+      </c>
+      <c r="I50" s="6">
+        <v>25</v>
+      </c>
+      <c r="O50" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="P50" s="6">
+        <v>65111</v>
+      </c>
+      <c r="Q50" s="6">
         <v>10</v>
       </c>
-      <c r="O47" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P47" s="1">
-        <v>45172</v>
-      </c>
-      <c r="Q47" s="1">
-        <v>9</v>
-      </c>
-      <c r="R47" s="1">
-        <v>141556</v>
-      </c>
-      <c r="S47" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B48" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="O48" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="P48" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q48" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="R48" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="S48" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B49" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D49" s="1" t="s">
+      <c r="R50" s="6">
+        <v>105485</v>
+      </c>
+      <c r="S50" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51" s="6">
+        <v>2016</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F51" s="6">
+        <v>60539</v>
+      </c>
+      <c r="G51" s="6">
+        <v>2</v>
+      </c>
+      <c r="H51" s="6">
+        <v>107661</v>
+      </c>
+      <c r="I51" s="6">
+        <v>8</v>
+      </c>
+      <c r="O51" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="P51" s="6">
+        <v>58728</v>
+      </c>
+      <c r="Q51" s="6">
+        <v>4</v>
+      </c>
+      <c r="R51" s="6">
+        <v>108275</v>
+      </c>
+      <c r="S51" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52" s="6">
+        <v>2016</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F52" s="6">
+        <v>78584</v>
+      </c>
+      <c r="G52" s="6">
+        <v>95</v>
+      </c>
+      <c r="H52" s="6">
+        <v>141277</v>
+      </c>
+      <c r="I52" s="6">
+        <v>124</v>
+      </c>
+      <c r="O52" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="P52" s="6">
+        <v>79167</v>
+      </c>
+      <c r="Q52" s="6">
+        <v>101</v>
+      </c>
+      <c r="R52" s="6">
+        <v>132460</v>
+      </c>
+      <c r="S52" s="6">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B53" s="6">
+        <v>2016</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F53" s="6">
+        <v>37602</v>
+      </c>
+      <c r="G53" s="6">
+        <v>28</v>
+      </c>
+      <c r="H53" s="6">
+        <v>180666</v>
+      </c>
+      <c r="I53" s="6">
+        <v>87</v>
+      </c>
+      <c r="O53" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="P53" s="6">
+        <v>43111</v>
+      </c>
+      <c r="Q53" s="6">
+        <v>43</v>
+      </c>
+      <c r="R53" s="6">
+        <v>166679</v>
+      </c>
+      <c r="S53" s="6">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B54" s="6">
+        <v>2016</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F54" s="6">
+        <v>46140</v>
+      </c>
+      <c r="G54" s="6">
+        <v>21</v>
+      </c>
+      <c r="H54" s="6">
+        <v>143964</v>
+      </c>
+      <c r="I54" s="6">
+        <v>81</v>
+      </c>
+      <c r="O54" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="P54" s="6">
+        <v>51710</v>
+      </c>
+      <c r="Q54" s="6">
+        <v>30</v>
+      </c>
+      <c r="R54" s="6">
+        <v>145267</v>
+      </c>
+      <c r="S54" s="6">
         <v>77</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F49" s="1">
-        <v>52390</v>
-      </c>
-      <c r="G49" s="1">
-        <v>14</v>
-      </c>
-      <c r="H49" s="1">
-        <v>101734</v>
-      </c>
-      <c r="I49" s="1">
+    </row>
+    <row r="55" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B55" s="6">
+        <v>2016</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F55" s="6">
+        <v>75842</v>
+      </c>
+      <c r="G55" s="6">
+        <v>10</v>
+      </c>
+      <c r="H55" s="6">
+        <v>113078</v>
+      </c>
+      <c r="I55" s="6">
+        <v>118</v>
+      </c>
+      <c r="O55" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="P55" s="6">
+        <v>75120</v>
+      </c>
+      <c r="Q55" s="6">
+        <v>18</v>
+      </c>
+      <c r="R55" s="6">
+        <v>116811</v>
+      </c>
+      <c r="S55" s="6">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B56" s="6">
+        <v>2016</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D56" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="O49" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P49" s="1">
-        <v>63288</v>
-      </c>
-      <c r="Q49" s="1">
-        <v>21</v>
-      </c>
-      <c r="R49" s="1">
-        <v>96934</v>
-      </c>
-      <c r="S49" s="1">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B50" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F50" s="1">
-        <v>64399</v>
-      </c>
-      <c r="G50" s="1">
-        <v>16</v>
-      </c>
-      <c r="H50" s="1">
-        <v>111679</v>
-      </c>
-      <c r="I50" s="1">
-        <v>25</v>
-      </c>
-      <c r="O50" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P50" s="1">
-        <v>65111</v>
-      </c>
-      <c r="Q50" s="1">
-        <v>10</v>
-      </c>
-      <c r="R50" s="1">
-        <v>105485</v>
-      </c>
-      <c r="S50" s="1">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B51" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F51" s="1">
-        <v>60539</v>
-      </c>
-      <c r="G51" s="1">
-        <v>2</v>
-      </c>
-      <c r="H51" s="1">
-        <v>107661</v>
-      </c>
-      <c r="I51" s="1">
-        <v>8</v>
-      </c>
-      <c r="O51" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="P51" s="1">
-        <v>58728</v>
-      </c>
-      <c r="Q51" s="1">
-        <v>4</v>
-      </c>
-      <c r="R51" s="1">
-        <v>108275</v>
-      </c>
-      <c r="S51" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B52" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F52" s="1">
-        <v>78584</v>
-      </c>
-      <c r="G52" s="1">
-        <v>95</v>
-      </c>
-      <c r="H52" s="1">
-        <v>141277</v>
-      </c>
-      <c r="I52" s="1">
-        <v>124</v>
-      </c>
-      <c r="O52" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P52" s="1">
-        <v>79167</v>
-      </c>
-      <c r="Q52" s="1">
-        <v>101</v>
-      </c>
-      <c r="R52" s="1">
-        <v>132460</v>
-      </c>
-      <c r="S52" s="1">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B53" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F53" s="1">
-        <v>37602</v>
-      </c>
-      <c r="G53" s="1">
-        <v>28</v>
-      </c>
-      <c r="H53" s="1">
-        <v>180666</v>
-      </c>
-      <c r="I53" s="1">
-        <v>87</v>
-      </c>
-      <c r="O53" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="P53" s="1">
-        <v>43111</v>
-      </c>
-      <c r="Q53" s="1">
-        <v>43</v>
-      </c>
-      <c r="R53" s="1">
-        <v>166679</v>
-      </c>
-      <c r="S53" s="1">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B54" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F54" s="1">
-        <v>46140</v>
-      </c>
-      <c r="G54" s="1">
-        <v>21</v>
-      </c>
-      <c r="H54" s="1">
-        <v>143964</v>
-      </c>
-      <c r="I54" s="1">
-        <v>81</v>
-      </c>
-      <c r="O54" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="P54" s="1">
-        <v>51710</v>
-      </c>
-      <c r="Q54" s="1">
-        <v>30</v>
-      </c>
-      <c r="R54" s="1">
-        <v>145267</v>
-      </c>
-      <c r="S54" s="1">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B55" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F55" s="1">
-        <v>75842</v>
-      </c>
-      <c r="G55" s="1">
-        <v>10</v>
-      </c>
-      <c r="H55" s="1">
-        <v>113078</v>
-      </c>
-      <c r="I55" s="1">
-        <v>118</v>
-      </c>
-      <c r="O55" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="P55" s="1">
-        <v>75120</v>
-      </c>
-      <c r="Q55" s="1">
-        <v>18</v>
-      </c>
-      <c r="R55" s="1">
-        <v>116811</v>
-      </c>
-      <c r="S55" s="1">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B56" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F56" s="1">
+      <c r="E56" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F56" s="6">
         <v>50086</v>
       </c>
-      <c r="G56" s="1">
+      <c r="G56" s="6">
         <v>34</v>
       </c>
-      <c r="H56" s="1">
+      <c r="H56" s="6">
         <v>143173</v>
       </c>
-      <c r="I56" s="1">
+      <c r="I56" s="6">
         <v>116</v>
       </c>
-      <c r="O56" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="P56" s="1">
+      <c r="O56" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="P56" s="6">
         <v>55340</v>
       </c>
-      <c r="Q56" s="1">
+      <c r="Q56" s="6">
         <v>49</v>
       </c>
-      <c r="R56" s="1">
+      <c r="R56" s="6">
         <v>148063</v>
       </c>
-      <c r="S56" s="1">
+      <c r="S56" s="6">
         <v>132</v>
       </c>
     </row>
@@ -3388,10 +3399,10 @@
         <v>2016</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>67</v>
@@ -3432,10 +3443,10 @@
         <v>2016</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>67</v>
@@ -3476,10 +3487,10 @@
         <v>2016</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>67</v>
@@ -3520,10 +3531,10 @@
         <v>2016</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>67</v>
@@ -3564,10 +3575,10 @@
         <v>2016</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>67</v>
@@ -3608,10 +3619,10 @@
         <v>2016</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>66</v>
@@ -3652,10 +3663,10 @@
         <v>2016</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>66</v>
@@ -3696,10 +3707,10 @@
         <v>2016</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>66</v>
@@ -3740,10 +3751,10 @@
         <v>2016</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>67</v>
@@ -3784,10 +3795,10 @@
         <v>2016</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>67</v>
@@ -3828,10 +3839,10 @@
         <v>2016</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>67</v>
@@ -3872,10 +3883,10 @@
         <v>2016</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>66</v>
@@ -3916,10 +3927,10 @@
         <v>2016</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>67</v>
@@ -3960,10 +3971,10 @@
         <v>2016</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>66</v>
@@ -4004,10 +4015,10 @@
         <v>2016</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>66</v>
@@ -4048,10 +4059,10 @@
         <v>2016</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>67</v>
@@ -4092,10 +4103,10 @@
         <v>2016</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>67</v>
@@ -4136,10 +4147,10 @@
         <v>2016</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>66</v>
@@ -4180,10 +4191,10 @@
         <v>2016</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>66</v>
@@ -4224,10 +4235,10 @@
         <v>2016</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>67</v>
@@ -4268,10 +4279,10 @@
         <v>2016</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>67</v>
@@ -4312,10 +4323,10 @@
         <v>2016</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>66</v>
@@ -4356,10 +4367,10 @@
         <v>2016</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>66</v>
@@ -4400,40 +4411,40 @@
         <v>2016</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O80" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P80" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q80" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R80" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S80" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.3">
@@ -4444,10 +4455,10 @@
         <v>2016</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>67</v>
@@ -4488,10 +4499,10 @@
         <v>2016</v>
       </c>
       <c r="C82" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>66</v>
@@ -4532,10 +4543,10 @@
         <v>2016</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>66</v>
@@ -4576,10 +4587,10 @@
         <v>2016</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>67</v>
@@ -4620,10 +4631,10 @@
         <v>2016</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>66</v>
@@ -4664,10 +4675,10 @@
         <v>2016</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>66</v>
@@ -4708,10 +4719,10 @@
         <v>2016</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>66</v>
@@ -4752,10 +4763,10 @@
         <v>2016</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>66</v>
@@ -4796,10 +4807,10 @@
         <v>2016</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>67</v>
@@ -4840,10 +4851,10 @@
         <v>2016</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>66</v>
@@ -4884,10 +4895,10 @@
         <v>2016</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>66</v>
@@ -4928,10 +4939,10 @@
         <v>2016</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>66</v>
@@ -4972,10 +4983,10 @@
         <v>2016</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>67</v>
@@ -5016,10 +5027,10 @@
         <v>2016</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>67</v>
@@ -5060,40 +5071,40 @@
         <v>2016</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O95" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P95" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q95" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R95" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S95" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.3">
@@ -5104,10 +5115,10 @@
         <v>2016</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>67</v>
@@ -5148,10 +5159,10 @@
         <v>2016</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>67</v>
@@ -5192,10 +5203,10 @@
         <v>2016</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>67</v>
@@ -5236,40 +5247,40 @@
         <v>2016</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O99" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P99" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q99" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R99" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S99" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.3">
@@ -5280,10 +5291,10 @@
         <v>2016</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>66</v>
@@ -5324,10 +5335,10 @@
         <v>2016</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>67</v>
@@ -5368,10 +5379,10 @@
         <v>2016</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>67</v>
@@ -5412,10 +5423,10 @@
         <v>2016</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>67</v>
@@ -5456,10 +5467,10 @@
         <v>2016</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>67</v>
@@ -5500,10 +5511,10 @@
         <v>2016</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>67</v>
@@ -5544,10 +5555,10 @@
         <v>2016</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>66</v>
@@ -5588,40 +5599,40 @@
         <v>2016</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O107" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P107" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q107" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R107" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S107" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="108" spans="1:19" x14ac:dyDescent="0.3">
@@ -5632,10 +5643,10 @@
         <v>2016</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>66</v>
@@ -5676,10 +5687,10 @@
         <v>2016</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>67</v>
@@ -5720,10 +5731,10 @@
         <v>2016</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>67</v>
@@ -5764,10 +5775,10 @@
         <v>2016</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>67</v>
@@ -5808,10 +5819,10 @@
         <v>2016</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>66</v>
@@ -5852,40 +5863,40 @@
         <v>2016</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O113" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P113" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q113" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R113" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S113" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.3">
@@ -5896,10 +5907,10 @@
         <v>2016</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>67</v>
@@ -5940,10 +5951,10 @@
         <v>2016</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>66</v>
@@ -5984,10 +5995,10 @@
         <v>2016</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>67</v>
@@ -6028,10 +6039,10 @@
         <v>2016</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>66</v>
@@ -6072,10 +6083,10 @@
         <v>2016</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>67</v>
@@ -6116,40 +6127,40 @@
         <v>2016</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O119" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P119" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q119" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R119" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S119" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.3">
@@ -6160,40 +6171,40 @@
         <v>2016</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O120" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="P120" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q120" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R120" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S120" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="121" spans="1:19" x14ac:dyDescent="0.3">
@@ -6204,10 +6215,10 @@
         <v>2016</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>66</v>
@@ -6249,23 +6260,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28508D30-A5BD-4EFE-B24D-76D052DE43B5}">
-  <dimension ref="A4:F4"/>
+  <dimension ref="A4:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>68</v>
+        <v>151</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Run 10 to embryo ionocyte data sheet
</commit_message>
<xml_diff>
--- a/Ionocyte/All embryo ionocyte data.xlsx
+++ b/Ionocyte/All embryo ionocyte data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teres\Documents\GitHub\MenidiaOA\Ionocyte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BECC014-9EB4-453D-856A-7509769C1B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4850ACFD-3697-439F-A303-2E23C6D39C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DAFCA9E7-78AB-4FDC-8B4B-32C2729B4956}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="195">
   <si>
     <t>Experiment</t>
   </si>
@@ -493,7 +493,133 @@
     <t xml:space="preserve">Used Frisk lab microscope. Units are already µm^2, skip for conversion from pixels. </t>
   </si>
   <si>
-    <t xml:space="preserve">Used dissecting microscope. Pixel sizes are different from the other samples. </t>
+    <t xml:space="preserve">Used dissecting microscope. Pixel sizes are different from the other samples. See Google Sheets notes sections of counting data. </t>
+  </si>
+  <si>
+    <t>run10</t>
+  </si>
+  <si>
+    <t>exp3</t>
+  </si>
+  <si>
+    <t>2016-346</t>
+  </si>
+  <si>
+    <t>2016-347</t>
+  </si>
+  <si>
+    <t>2016-348</t>
+  </si>
+  <si>
+    <t>2016-349</t>
+  </si>
+  <si>
+    <t>2016-351</t>
+  </si>
+  <si>
+    <t>2016-352</t>
+  </si>
+  <si>
+    <t>2016-353</t>
+  </si>
+  <si>
+    <t>2016-354</t>
+  </si>
+  <si>
+    <t>2016-355</t>
+  </si>
+  <si>
+    <t>2016-356</t>
+  </si>
+  <si>
+    <t>2016-357</t>
+  </si>
+  <si>
+    <t>2016-358</t>
+  </si>
+  <si>
+    <t>2016-359</t>
+  </si>
+  <si>
+    <t>2016-360</t>
+  </si>
+  <si>
+    <t>2016-361</t>
+  </si>
+  <si>
+    <t>2016-362</t>
+  </si>
+  <si>
+    <t>2016-363</t>
+  </si>
+  <si>
+    <t>2016-364</t>
+  </si>
+  <si>
+    <t>2016-365</t>
+  </si>
+  <si>
+    <t>2016-366</t>
+  </si>
+  <si>
+    <t>2016-367</t>
+  </si>
+  <si>
+    <t>2016-368</t>
+  </si>
+  <si>
+    <t>2016-369</t>
+  </si>
+  <si>
+    <t>2016-370</t>
+  </si>
+  <si>
+    <t>2016-371</t>
+  </si>
+  <si>
+    <t>2016-372</t>
+  </si>
+  <si>
+    <t>2016-373</t>
+  </si>
+  <si>
+    <t>2016-374</t>
+  </si>
+  <si>
+    <t>2016-375</t>
+  </si>
+  <si>
+    <t>2016-376</t>
+  </si>
+  <si>
+    <t>2016-377</t>
+  </si>
+  <si>
+    <t>2016-378</t>
+  </si>
+  <si>
+    <t>2016-379</t>
+  </si>
+  <si>
+    <t>2016-380</t>
+  </si>
+  <si>
+    <t>2016-381</t>
+  </si>
+  <si>
+    <t>2016-382</t>
+  </si>
+  <si>
+    <t>2016-383</t>
+  </si>
+  <si>
+    <t>2016-384</t>
+  </si>
+  <si>
+    <t>2016-385</t>
+  </si>
+  <si>
+    <t>2016-350b</t>
   </si>
 </sst>
 </file>
@@ -884,11 +1010,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F1C880-24DC-4CF8-8C86-70B462FC0B54}">
-  <dimension ref="A1:X121"/>
+  <dimension ref="A1:X162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J157" sqref="J157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6251,6 +6377,1786 @@
         <v>32</v>
       </c>
     </row>
+    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B122" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F122" s="1">
+        <v>445914</v>
+      </c>
+      <c r="G122" s="1">
+        <v>41</v>
+      </c>
+      <c r="H122" s="1">
+        <v>629847</v>
+      </c>
+      <c r="I122" s="1">
+        <v>263</v>
+      </c>
+      <c r="O122" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P122" s="1">
+        <v>437484</v>
+      </c>
+      <c r="Q122" s="1">
+        <v>29</v>
+      </c>
+      <c r="R122" s="1">
+        <v>625352</v>
+      </c>
+      <c r="S122" s="1">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A123" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B123" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F123" s="1">
+        <v>439119</v>
+      </c>
+      <c r="G123" s="1">
+        <v>56</v>
+      </c>
+      <c r="H123" s="1">
+        <v>601111</v>
+      </c>
+      <c r="I123" s="1">
+        <v>72</v>
+      </c>
+      <c r="O123" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P123" s="1">
+        <v>415117</v>
+      </c>
+      <c r="Q123" s="1">
+        <v>44</v>
+      </c>
+      <c r="R123" s="1">
+        <v>689282</v>
+      </c>
+      <c r="S123" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B124" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F124" s="1">
+        <v>471980</v>
+      </c>
+      <c r="G124" s="1">
+        <v>53</v>
+      </c>
+      <c r="H124" s="1">
+        <v>752065</v>
+      </c>
+      <c r="I124" s="1">
+        <v>129</v>
+      </c>
+      <c r="O124" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P124" s="1">
+        <v>582087</v>
+      </c>
+      <c r="Q124" s="1">
+        <v>52</v>
+      </c>
+      <c r="R124" s="1">
+        <v>675424</v>
+      </c>
+      <c r="S124" s="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A125" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B125" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F125" s="1">
+        <v>497265</v>
+      </c>
+      <c r="G125" s="1">
+        <v>37</v>
+      </c>
+      <c r="H125" s="1">
+        <v>662060</v>
+      </c>
+      <c r="I125" s="1">
+        <v>47</v>
+      </c>
+      <c r="O125" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P125" s="1">
+        <v>482259</v>
+      </c>
+      <c r="Q125" s="1">
+        <v>34</v>
+      </c>
+      <c r="R125" s="1">
+        <v>671130</v>
+      </c>
+      <c r="S125" s="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A126" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B126" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F126" s="1">
+        <v>180830</v>
+      </c>
+      <c r="G126" s="1">
+        <v>42</v>
+      </c>
+      <c r="H126" s="1">
+        <v>821994</v>
+      </c>
+      <c r="I126" s="1">
+        <v>332</v>
+      </c>
+      <c r="O126" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P126" s="1">
+        <v>447670</v>
+      </c>
+      <c r="Q126" s="1">
+        <v>24</v>
+      </c>
+      <c r="R126" s="1">
+        <v>506851</v>
+      </c>
+      <c r="S126" s="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A127" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B127" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F127" s="1">
+        <v>346819</v>
+      </c>
+      <c r="G127" s="1">
+        <v>35</v>
+      </c>
+      <c r="H127" s="1">
+        <v>505157</v>
+      </c>
+      <c r="I127" s="1">
+        <v>92</v>
+      </c>
+      <c r="O127" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P127" s="1">
+        <v>351000</v>
+      </c>
+      <c r="Q127" s="1">
+        <v>40</v>
+      </c>
+      <c r="R127" s="1">
+        <v>517455</v>
+      </c>
+      <c r="S127" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A128" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B128" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F128" s="1">
+        <v>440393</v>
+      </c>
+      <c r="G128" s="1">
+        <v>13</v>
+      </c>
+      <c r="H128" s="1">
+        <v>593791</v>
+      </c>
+      <c r="I128" s="1">
+        <v>145</v>
+      </c>
+      <c r="O128" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P128" s="1">
+        <v>430513</v>
+      </c>
+      <c r="Q128" s="1">
+        <v>29</v>
+      </c>
+      <c r="R128" s="1">
+        <v>599207</v>
+      </c>
+      <c r="S128" s="1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A129" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B129" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F129" s="1">
+        <v>434107</v>
+      </c>
+      <c r="G129" s="1">
+        <v>40</v>
+      </c>
+      <c r="H129" s="1">
+        <v>597169</v>
+      </c>
+      <c r="I129" s="1">
+        <v>143</v>
+      </c>
+      <c r="O129" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P129" s="1">
+        <v>345909</v>
+      </c>
+      <c r="Q129" s="1">
+        <v>23</v>
+      </c>
+      <c r="R129" s="1">
+        <v>708847</v>
+      </c>
+      <c r="S129" s="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A130" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B130" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F130" s="1">
+        <v>353001</v>
+      </c>
+      <c r="G130" s="1">
+        <v>35</v>
+      </c>
+      <c r="H130" s="1">
+        <v>709241</v>
+      </c>
+      <c r="I130" s="1">
+        <v>192</v>
+      </c>
+      <c r="O130" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P130" s="1">
+        <v>370878</v>
+      </c>
+      <c r="Q130" s="1">
+        <v>47</v>
+      </c>
+      <c r="R130" s="1">
+        <v>685493</v>
+      </c>
+      <c r="S130" s="1">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B131" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F131" s="1">
+        <v>376745</v>
+      </c>
+      <c r="G131" s="1">
+        <v>40</v>
+      </c>
+      <c r="H131" s="1">
+        <v>605739</v>
+      </c>
+      <c r="I131" s="1">
+        <v>116</v>
+      </c>
+      <c r="O131" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P131" s="1">
+        <v>342820</v>
+      </c>
+      <c r="Q131" s="1">
+        <v>27</v>
+      </c>
+      <c r="R131" s="1">
+        <v>647238</v>
+      </c>
+      <c r="S131" s="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A132" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B132" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F132" s="1">
+        <v>378456</v>
+      </c>
+      <c r="G132" s="1">
+        <v>19</v>
+      </c>
+      <c r="H132" s="1">
+        <v>592160</v>
+      </c>
+      <c r="I132" s="1">
+        <v>73</v>
+      </c>
+      <c r="O132" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P132" s="1">
+        <v>374114</v>
+      </c>
+      <c r="Q132" s="1">
+        <v>7</v>
+      </c>
+      <c r="R132" s="1">
+        <v>601448</v>
+      </c>
+      <c r="S132" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A133" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B133" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F133" s="1">
+        <v>263390</v>
+      </c>
+      <c r="G133" s="1">
+        <v>3</v>
+      </c>
+      <c r="H133" s="1">
+        <v>714048</v>
+      </c>
+      <c r="I133" s="1">
+        <v>15</v>
+      </c>
+      <c r="O133" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P133" s="1">
+        <v>324369</v>
+      </c>
+      <c r="Q133" s="1">
+        <v>6</v>
+      </c>
+      <c r="R133" s="1">
+        <v>618676</v>
+      </c>
+      <c r="S133" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A134" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B134" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="O134" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="135" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A135" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B135" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F135" s="1">
+        <v>414032</v>
+      </c>
+      <c r="G135" s="1">
+        <v>35</v>
+      </c>
+      <c r="H135" s="1">
+        <v>556978</v>
+      </c>
+      <c r="I135" s="1">
+        <v>200</v>
+      </c>
+      <c r="O135" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P135" s="1">
+        <v>398022</v>
+      </c>
+      <c r="Q135" s="1">
+        <v>20</v>
+      </c>
+      <c r="R135" s="1">
+        <v>569898</v>
+      </c>
+      <c r="S135" s="1">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="136" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A136" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B136" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F136" s="1">
+        <v>247368</v>
+      </c>
+      <c r="G136" s="1">
+        <v>100</v>
+      </c>
+      <c r="H136" s="1">
+        <v>816536</v>
+      </c>
+      <c r="I136" s="1">
+        <v>163</v>
+      </c>
+      <c r="O136" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P136" s="1">
+        <v>388209</v>
+      </c>
+      <c r="Q136" s="1">
+        <v>23</v>
+      </c>
+      <c r="R136" s="1">
+        <v>630701</v>
+      </c>
+      <c r="S136" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="137" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A137" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B137" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F137" s="1">
+        <v>249383</v>
+      </c>
+      <c r="G137" s="1">
+        <v>32</v>
+      </c>
+      <c r="H137" s="1">
+        <v>613840</v>
+      </c>
+      <c r="I137" s="1">
+        <v>111</v>
+      </c>
+      <c r="O137" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P137" s="1">
+        <v>247674</v>
+      </c>
+      <c r="Q137" s="1">
+        <v>19</v>
+      </c>
+      <c r="R137" s="1">
+        <v>623427</v>
+      </c>
+      <c r="S137" s="1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="138" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A138" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B138" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F138" s="1">
+        <v>384613</v>
+      </c>
+      <c r="G138" s="1">
+        <v>48</v>
+      </c>
+      <c r="H138" s="1">
+        <v>602647</v>
+      </c>
+      <c r="I138" s="1">
+        <v>257</v>
+      </c>
+      <c r="O138" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P138" s="1">
+        <v>370068</v>
+      </c>
+      <c r="Q138" s="1">
+        <v>39</v>
+      </c>
+      <c r="R138" s="1">
+        <v>596280</v>
+      </c>
+      <c r="S138" s="1">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="139" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A139" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B139" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F139" s="1">
+        <v>303423</v>
+      </c>
+      <c r="G139" s="1">
+        <v>123</v>
+      </c>
+      <c r="H139" s="1">
+        <v>826282</v>
+      </c>
+      <c r="I139" s="1">
+        <v>341</v>
+      </c>
+      <c r="O139" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P139" s="1">
+        <v>268572</v>
+      </c>
+      <c r="Q139" s="1">
+        <v>135</v>
+      </c>
+      <c r="R139" s="1">
+        <v>772657</v>
+      </c>
+      <c r="S139" s="1">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="140" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A140" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B140" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F140" s="1">
+        <v>456140</v>
+      </c>
+      <c r="G140" s="1">
+        <v>9</v>
+      </c>
+      <c r="H140" s="1">
+        <v>548221</v>
+      </c>
+      <c r="I140" s="1">
+        <v>103</v>
+      </c>
+      <c r="O140" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P140" s="1">
+        <v>441150</v>
+      </c>
+      <c r="Q140" s="1">
+        <v>5</v>
+      </c>
+      <c r="R140" s="1">
+        <v>559663</v>
+      </c>
+      <c r="S140" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="141" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A141" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B141" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F141" s="1">
+        <v>398605</v>
+      </c>
+      <c r="G141" s="1">
+        <v>25</v>
+      </c>
+      <c r="H141" s="1">
+        <v>612751</v>
+      </c>
+      <c r="I141" s="1">
+        <v>82</v>
+      </c>
+      <c r="O141" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P141" s="1">
+        <v>363837</v>
+      </c>
+      <c r="Q141" s="1">
+        <v>12</v>
+      </c>
+      <c r="R141" s="1">
+        <v>640813</v>
+      </c>
+      <c r="S141" s="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="142" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A142" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B142" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F142" s="1">
+        <v>388685</v>
+      </c>
+      <c r="G142" s="1">
+        <v>16</v>
+      </c>
+      <c r="H142" s="1">
+        <v>530675</v>
+      </c>
+      <c r="I142" s="1">
+        <v>43</v>
+      </c>
+      <c r="O142" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P142" s="1">
+        <v>403154</v>
+      </c>
+      <c r="Q142" s="1">
+        <v>17</v>
+      </c>
+      <c r="R142" s="1">
+        <v>517357</v>
+      </c>
+      <c r="S142" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="143" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A143" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B143" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F143" s="1">
+        <v>469710</v>
+      </c>
+      <c r="G143" s="1">
+        <v>19</v>
+      </c>
+      <c r="H143" s="1">
+        <v>494802</v>
+      </c>
+      <c r="I143" s="1">
+        <v>48</v>
+      </c>
+      <c r="O143" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P143" s="1">
+        <v>502152</v>
+      </c>
+      <c r="Q143" s="1">
+        <v>11</v>
+      </c>
+      <c r="R143" s="1">
+        <v>463162</v>
+      </c>
+      <c r="S143" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="144" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A144" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B144" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F144" s="1">
+        <v>357195</v>
+      </c>
+      <c r="G144" s="1">
+        <v>38</v>
+      </c>
+      <c r="H144" s="1">
+        <v>627888</v>
+      </c>
+      <c r="I144" s="1">
+        <v>119</v>
+      </c>
+      <c r="O144" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P144" s="1">
+        <v>406042</v>
+      </c>
+      <c r="Q144" s="1">
+        <v>65</v>
+      </c>
+      <c r="R144" s="1">
+        <v>505226</v>
+      </c>
+      <c r="S144" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="145" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A145" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B145" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F145" s="1">
+        <v>326842</v>
+      </c>
+      <c r="G145" s="1">
+        <v>72</v>
+      </c>
+      <c r="H145" s="1">
+        <v>1010451</v>
+      </c>
+      <c r="I145" s="1">
+        <v>242</v>
+      </c>
+      <c r="O145" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P145" s="1">
+        <v>396661</v>
+      </c>
+      <c r="Q145" s="1">
+        <v>61</v>
+      </c>
+      <c r="R145" s="1">
+        <v>623519</v>
+      </c>
+      <c r="S145" s="1">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="146" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A146" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B146" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F146" s="1">
+        <v>410124</v>
+      </c>
+      <c r="G146" s="1">
+        <v>30</v>
+      </c>
+      <c r="H146" s="1">
+        <v>640876</v>
+      </c>
+      <c r="I146" s="1">
+        <v>101</v>
+      </c>
+      <c r="O146" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P146" s="1">
+        <v>407983</v>
+      </c>
+      <c r="Q146" s="1">
+        <v>25</v>
+      </c>
+      <c r="R146" s="1">
+        <v>635056</v>
+      </c>
+      <c r="S146" s="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="147" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A147" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B147" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F147" s="1">
+        <v>265711</v>
+      </c>
+      <c r="G147" s="1">
+        <v>33</v>
+      </c>
+      <c r="H147" s="1">
+        <v>714559</v>
+      </c>
+      <c r="I147" s="1">
+        <v>145</v>
+      </c>
+      <c r="O147" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P147" s="1">
+        <v>265899</v>
+      </c>
+      <c r="Q147" s="1">
+        <v>25</v>
+      </c>
+      <c r="R147" s="1">
+        <v>446936</v>
+      </c>
+      <c r="S147" s="1">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="148" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A148" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B148" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F148" s="1">
+        <v>347908</v>
+      </c>
+      <c r="G148" s="1">
+        <v>24</v>
+      </c>
+      <c r="H148" s="1">
+        <v>544126</v>
+      </c>
+      <c r="I148" s="1">
+        <v>73</v>
+      </c>
+      <c r="O148" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P148" s="1">
+        <v>329765</v>
+      </c>
+      <c r="Q148" s="1">
+        <v>23</v>
+      </c>
+      <c r="R148" s="1">
+        <v>565934</v>
+      </c>
+      <c r="S148" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="149" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A149" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B149" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F149" s="1">
+        <v>377552</v>
+      </c>
+      <c r="G149" s="1">
+        <v>88</v>
+      </c>
+      <c r="H149" s="1">
+        <v>616446</v>
+      </c>
+      <c r="I149" s="1">
+        <v>92</v>
+      </c>
+      <c r="O149" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P149" s="1">
+        <v>380134</v>
+      </c>
+      <c r="Q149" s="1">
+        <v>64</v>
+      </c>
+      <c r="R149" s="1">
+        <v>611068</v>
+      </c>
+      <c r="S149" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="150" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A150" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B150" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F150" s="1">
+        <v>255808</v>
+      </c>
+      <c r="G150" s="1">
+        <v>128</v>
+      </c>
+      <c r="H150" s="1">
+        <v>758602</v>
+      </c>
+      <c r="I150" s="1">
+        <v>111</v>
+      </c>
+      <c r="O150" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P150" s="1">
+        <v>411130</v>
+      </c>
+      <c r="Q150" s="1">
+        <v>28</v>
+      </c>
+      <c r="R150" s="1">
+        <v>557750</v>
+      </c>
+      <c r="S150" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="151" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A151" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B151" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F151" s="1">
+        <v>341633</v>
+      </c>
+      <c r="G151" s="1">
+        <v>46</v>
+      </c>
+      <c r="H151" s="1">
+        <v>669826</v>
+      </c>
+      <c r="I151" s="1">
+        <v>181</v>
+      </c>
+      <c r="O151" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P151" s="1">
+        <v>330053</v>
+      </c>
+      <c r="Q151" s="1">
+        <v>40</v>
+      </c>
+      <c r="R151" s="1">
+        <v>684589</v>
+      </c>
+      <c r="S151" s="1">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="152" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A152" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B152" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F152" s="1">
+        <v>400939</v>
+      </c>
+      <c r="G152" s="1">
+        <v>82</v>
+      </c>
+      <c r="H152" s="1">
+        <v>592315</v>
+      </c>
+      <c r="I152" s="1">
+        <v>224</v>
+      </c>
+      <c r="O152" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P152" s="1">
+        <v>398230</v>
+      </c>
+      <c r="Q152" s="1">
+        <v>65</v>
+      </c>
+      <c r="R152" s="1">
+        <v>591949</v>
+      </c>
+      <c r="S152" s="1">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="153" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A153" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B153" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F153" s="1">
+        <v>269327</v>
+      </c>
+      <c r="G153" s="1">
+        <v>26</v>
+      </c>
+      <c r="H153" s="1">
+        <v>448409</v>
+      </c>
+      <c r="I153" s="1">
+        <v>140</v>
+      </c>
+      <c r="O153" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P153" s="1">
+        <v>323362</v>
+      </c>
+      <c r="Q153" s="1">
+        <v>16</v>
+      </c>
+      <c r="R153" s="1">
+        <v>537303</v>
+      </c>
+      <c r="S153" s="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="154" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A154" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B154" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F154" s="1">
+        <v>284360</v>
+      </c>
+      <c r="G154" s="1">
+        <v>44</v>
+      </c>
+      <c r="H154" s="1">
+        <v>458012</v>
+      </c>
+      <c r="I154" s="1">
+        <v>167</v>
+      </c>
+      <c r="O154" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P154" s="1">
+        <v>322120</v>
+      </c>
+      <c r="Q154" s="1">
+        <v>15</v>
+      </c>
+      <c r="R154" s="1">
+        <v>562980</v>
+      </c>
+      <c r="S154" s="1">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="155" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A155" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B155" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F155" s="1">
+        <v>278404</v>
+      </c>
+      <c r="G155" s="1">
+        <v>65</v>
+      </c>
+      <c r="H155" s="1">
+        <v>604847</v>
+      </c>
+      <c r="I155" s="1">
+        <v>188</v>
+      </c>
+      <c r="O155" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P155" s="1">
+        <v>437086</v>
+      </c>
+      <c r="Q155" s="1">
+        <v>17</v>
+      </c>
+      <c r="R155" s="1">
+        <v>509499</v>
+      </c>
+      <c r="S155" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="156" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A156" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B156" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F156" s="1">
+        <v>327605</v>
+      </c>
+      <c r="G156" s="1">
+        <v>51</v>
+      </c>
+      <c r="H156" s="1">
+        <v>436479</v>
+      </c>
+      <c r="I156" s="1">
+        <v>87</v>
+      </c>
+      <c r="O156" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P156" s="1">
+        <v>418853</v>
+      </c>
+      <c r="Q156" s="1">
+        <v>26</v>
+      </c>
+      <c r="R156" s="1">
+        <v>584861</v>
+      </c>
+      <c r="S156" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="157" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A157" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B157" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F157" s="1">
+        <v>300451</v>
+      </c>
+      <c r="G157" s="1">
+        <v>56</v>
+      </c>
+      <c r="H157" s="1">
+        <v>75885</v>
+      </c>
+      <c r="I157" s="1">
+        <v>93</v>
+      </c>
+      <c r="O157" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P157" s="1">
+        <v>333377</v>
+      </c>
+      <c r="Q157" s="1">
+        <v>32</v>
+      </c>
+      <c r="R157" s="1">
+        <v>591410</v>
+      </c>
+      <c r="S157" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="158" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A158" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B158" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F158" s="1">
+        <v>379743</v>
+      </c>
+      <c r="G158" s="1">
+        <v>59</v>
+      </c>
+      <c r="H158" s="1">
+        <v>595622</v>
+      </c>
+      <c r="I158" s="1">
+        <v>157</v>
+      </c>
+      <c r="O158" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P158" s="1">
+        <v>429754</v>
+      </c>
+      <c r="Q158" s="1">
+        <v>45</v>
+      </c>
+      <c r="R158" s="1">
+        <v>697052</v>
+      </c>
+      <c r="S158" s="1">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="159" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A159" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B159" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F159" s="1">
+        <v>265874</v>
+      </c>
+      <c r="G159" s="1">
+        <v>41</v>
+      </c>
+      <c r="H159" s="1">
+        <v>494014</v>
+      </c>
+      <c r="I159" s="1">
+        <v>112</v>
+      </c>
+      <c r="O159" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P159" s="1">
+        <v>294833</v>
+      </c>
+      <c r="Q159" s="1">
+        <v>29</v>
+      </c>
+      <c r="R159" s="1">
+        <v>574812</v>
+      </c>
+      <c r="S159" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="160" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A160" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B160" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F160" s="1">
+        <v>384285</v>
+      </c>
+      <c r="G160" s="1">
+        <v>115</v>
+      </c>
+      <c r="H160" s="1">
+        <v>477438</v>
+      </c>
+      <c r="I160" s="1">
+        <v>111</v>
+      </c>
+      <c r="O160" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P160" s="1">
+        <v>404663</v>
+      </c>
+      <c r="Q160" s="1">
+        <v>103</v>
+      </c>
+      <c r="R160" s="1">
+        <v>475347</v>
+      </c>
+      <c r="S160" s="1">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="161" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A161" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B161" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F161" s="1">
+        <v>378654</v>
+      </c>
+      <c r="G161" s="1">
+        <v>53</v>
+      </c>
+      <c r="H161" s="1">
+        <v>491376</v>
+      </c>
+      <c r="I161" s="1">
+        <v>118</v>
+      </c>
+      <c r="O161" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P161" s="1">
+        <v>378677</v>
+      </c>
+      <c r="Q161" s="1">
+        <v>21</v>
+      </c>
+      <c r="R161" s="1">
+        <v>498724</v>
+      </c>
+      <c r="S161" s="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="162" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A162" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B162" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F162" s="1">
+        <v>275287</v>
+      </c>
+      <c r="G162" s="1">
+        <v>35</v>
+      </c>
+      <c r="H162" s="1">
+        <v>622852</v>
+      </c>
+      <c r="I162" s="1">
+        <v>111</v>
+      </c>
+      <c r="O162" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P162" s="1">
+        <v>281322</v>
+      </c>
+      <c r="Q162" s="1">
+        <v>38</v>
+      </c>
+      <c r="R162" s="1">
+        <v>617180</v>
+      </c>
+      <c r="S162" s="1">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6260,15 +8166,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28508D30-A5BD-4EFE-B24D-76D052DE43B5}">
-  <dimension ref="A4:H6"/>
+  <dimension ref="A4:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>151</v>
       </c>
@@ -6280,7 +8186,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>152</v>
       </c>
@@ -6291,6 +8197,10 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added runs 10 and 12 to embryo ionocyte data
</commit_message>
<xml_diff>
--- a/Ionocyte/All embryo ionocyte data.xlsx
+++ b/Ionocyte/All embryo ionocyte data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teres\Documents\GitHub\MenidiaOA\Ionocyte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4850ACFD-3697-439F-A303-2E23C6D39C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900ED4AE-1CD4-4FF6-A743-5260D91CCE23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DAFCA9E7-78AB-4FDC-8B4B-32C2729B4956}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="277">
   <si>
     <t>Experiment</t>
   </si>
@@ -620,6 +620,252 @@
   </si>
   <si>
     <t>2016-350b</t>
+  </si>
+  <si>
+    <t>run12</t>
+  </si>
+  <si>
+    <t>2016-426</t>
+  </si>
+  <si>
+    <t>2016-427</t>
+  </si>
+  <si>
+    <t>2016-428</t>
+  </si>
+  <si>
+    <t>2016-429</t>
+  </si>
+  <si>
+    <t>2016-430</t>
+  </si>
+  <si>
+    <t>2016-431</t>
+  </si>
+  <si>
+    <t>2016-432</t>
+  </si>
+  <si>
+    <t>2016-433</t>
+  </si>
+  <si>
+    <t>2016-434</t>
+  </si>
+  <si>
+    <t>2016-435</t>
+  </si>
+  <si>
+    <t>2016-436</t>
+  </si>
+  <si>
+    <t>2016-437</t>
+  </si>
+  <si>
+    <t>2016-438</t>
+  </si>
+  <si>
+    <t>2016-439</t>
+  </si>
+  <si>
+    <t>2016-440</t>
+  </si>
+  <si>
+    <t>2016-441</t>
+  </si>
+  <si>
+    <t>2016-442</t>
+  </si>
+  <si>
+    <t>2016-443</t>
+  </si>
+  <si>
+    <t>2016-444</t>
+  </si>
+  <si>
+    <t>2016-445</t>
+  </si>
+  <si>
+    <t>2016-446</t>
+  </si>
+  <si>
+    <t>2016-447</t>
+  </si>
+  <si>
+    <t>2016-448</t>
+  </si>
+  <si>
+    <t>2016-449</t>
+  </si>
+  <si>
+    <t>2016-450</t>
+  </si>
+  <si>
+    <t>2016-451</t>
+  </si>
+  <si>
+    <t>2016-452</t>
+  </si>
+  <si>
+    <t>2016-453</t>
+  </si>
+  <si>
+    <t>2016-454</t>
+  </si>
+  <si>
+    <t>2016-455</t>
+  </si>
+  <si>
+    <t>2016-456</t>
+  </si>
+  <si>
+    <t>2016-457</t>
+  </si>
+  <si>
+    <t>2016-458</t>
+  </si>
+  <si>
+    <t>2016-459</t>
+  </si>
+  <si>
+    <t>2016-460</t>
+  </si>
+  <si>
+    <t>2016-461</t>
+  </si>
+  <si>
+    <t>2016-462</t>
+  </si>
+  <si>
+    <t>2016-463</t>
+  </si>
+  <si>
+    <t>2016-464</t>
+  </si>
+  <si>
+    <t>2016-465</t>
+  </si>
+  <si>
+    <t>run14</t>
+  </si>
+  <si>
+    <t>2016-506</t>
+  </si>
+  <si>
+    <t>2016-507</t>
+  </si>
+  <si>
+    <t>2016-509</t>
+  </si>
+  <si>
+    <t>2016-510</t>
+  </si>
+  <si>
+    <t>2016-511</t>
+  </si>
+  <si>
+    <t>2016-512</t>
+  </si>
+  <si>
+    <t>2016-513</t>
+  </si>
+  <si>
+    <t>2016-514</t>
+  </si>
+  <si>
+    <t>2016-515</t>
+  </si>
+  <si>
+    <t>2016-516</t>
+  </si>
+  <si>
+    <t>2016-517</t>
+  </si>
+  <si>
+    <t>2016-518</t>
+  </si>
+  <si>
+    <t>2016-519</t>
+  </si>
+  <si>
+    <t>2016-520</t>
+  </si>
+  <si>
+    <t>2016-521</t>
+  </si>
+  <si>
+    <t>2016-522</t>
+  </si>
+  <si>
+    <t>2016-523</t>
+  </si>
+  <si>
+    <t>2016-524</t>
+  </si>
+  <si>
+    <t>2016-525</t>
+  </si>
+  <si>
+    <t>2016-526</t>
+  </si>
+  <si>
+    <t>2016-527</t>
+  </si>
+  <si>
+    <t>2016-528</t>
+  </si>
+  <si>
+    <t>2016-529</t>
+  </si>
+  <si>
+    <t>2016-530</t>
+  </si>
+  <si>
+    <t>2016-531</t>
+  </si>
+  <si>
+    <t>2016-532</t>
+  </si>
+  <si>
+    <t>2016-533</t>
+  </si>
+  <si>
+    <t>2016-534</t>
+  </si>
+  <si>
+    <t>2016-535</t>
+  </si>
+  <si>
+    <t>2016-536</t>
+  </si>
+  <si>
+    <t>2016-537</t>
+  </si>
+  <si>
+    <t>2016-538</t>
+  </si>
+  <si>
+    <t>2016-539</t>
+  </si>
+  <si>
+    <t>2016-540</t>
+  </si>
+  <si>
+    <t>2016-541</t>
+  </si>
+  <si>
+    <t>2016-542</t>
+  </si>
+  <si>
+    <t>2016-543</t>
+  </si>
+  <si>
+    <t>2016-544</t>
+  </si>
+  <si>
+    <t>2016-545</t>
+  </si>
+  <si>
+    <t>2016-546</t>
   </si>
 </sst>
 </file>
@@ -655,7 +901,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -674,6 +920,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -687,7 +939,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -696,6 +948,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1010,11 +1263,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F1C880-24DC-4CF8-8C86-70B462FC0B54}">
-  <dimension ref="A1:X162"/>
+  <dimension ref="A1:X243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J157" sqref="J157"/>
+      <pane ySplit="1" topLeftCell="A195" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D205" sqref="D205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6921,7 +7174,31 @@
       <c r="E134" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="F134" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H134" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I134" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="O134" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P134" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q134" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R134" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="S134" s="1" t="s">
         <v>109</v>
       </c>
     </row>
@@ -8155,6 +8432,2370 @@
       </c>
       <c r="S162" s="1">
         <v>90</v>
+      </c>
+    </row>
+    <row r="163" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A163" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B163" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F163" s="1">
+        <v>264524</v>
+      </c>
+      <c r="G163" s="1">
+        <v>52</v>
+      </c>
+      <c r="H163" s="1">
+        <v>585854</v>
+      </c>
+      <c r="I163" s="1">
+        <v>233</v>
+      </c>
+      <c r="O163" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P163" s="1">
+        <v>315654</v>
+      </c>
+      <c r="Q163" s="1">
+        <v>49</v>
+      </c>
+      <c r="R163" s="1">
+        <v>569748</v>
+      </c>
+      <c r="S163" s="1">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="164" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A164" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B164" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F164" s="1">
+        <v>261511</v>
+      </c>
+      <c r="G164" s="1">
+        <v>88</v>
+      </c>
+      <c r="H164" s="1">
+        <v>669441</v>
+      </c>
+      <c r="I164" s="1">
+        <v>303</v>
+      </c>
+      <c r="O164" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P164" s="1">
+        <v>268050</v>
+      </c>
+      <c r="Q164" s="1">
+        <v>32</v>
+      </c>
+      <c r="R164" s="1">
+        <v>672110</v>
+      </c>
+      <c r="S164" s="1">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="165" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A165" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B165" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F165" s="1">
+        <v>496598</v>
+      </c>
+      <c r="G165" s="1">
+        <v>87</v>
+      </c>
+      <c r="H165" s="1">
+        <v>524587</v>
+      </c>
+      <c r="I165" s="1">
+        <v>210</v>
+      </c>
+      <c r="O165" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P165" s="1">
+        <v>471043</v>
+      </c>
+      <c r="Q165" s="1">
+        <v>55</v>
+      </c>
+      <c r="R165" s="1">
+        <v>567169</v>
+      </c>
+      <c r="S165" s="1">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="166" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A166" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B166" s="8">
+        <v>2016</v>
+      </c>
+      <c r="C166" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D166" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="E166" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F166" s="8">
+        <v>0</v>
+      </c>
+      <c r="G166" s="8">
+        <v>0</v>
+      </c>
+      <c r="H166" s="8">
+        <v>941871</v>
+      </c>
+      <c r="I166" s="8">
+        <v>417</v>
+      </c>
+      <c r="O166" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="P166" s="8">
+        <v>50892</v>
+      </c>
+      <c r="Q166" s="8">
+        <v>20</v>
+      </c>
+      <c r="R166" s="8">
+        <v>868618</v>
+      </c>
+      <c r="S166" s="8">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="167" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A167" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B167" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F167" s="1">
+        <v>279780</v>
+      </c>
+      <c r="G167" s="1">
+        <v>65</v>
+      </c>
+      <c r="H167" s="1">
+        <v>689215</v>
+      </c>
+      <c r="I167" s="1">
+        <v>266</v>
+      </c>
+      <c r="O167" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P167" s="1">
+        <v>288027</v>
+      </c>
+      <c r="Q167" s="1">
+        <v>37</v>
+      </c>
+      <c r="R167" s="1">
+        <v>686867</v>
+      </c>
+      <c r="S167" s="1">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="168" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A168" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B168" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F168" s="1">
+        <v>294780</v>
+      </c>
+      <c r="G168" s="1">
+        <v>152</v>
+      </c>
+      <c r="H168" s="1">
+        <v>619815</v>
+      </c>
+      <c r="I168" s="1">
+        <v>305</v>
+      </c>
+      <c r="O168" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P168" s="1">
+        <v>253074</v>
+      </c>
+      <c r="Q168" s="1">
+        <v>51</v>
+      </c>
+      <c r="R168" s="1">
+        <v>688324</v>
+      </c>
+      <c r="S168" s="1">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="169" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A169" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B169" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F169" s="1">
+        <v>279744</v>
+      </c>
+      <c r="G169" s="1">
+        <v>70</v>
+      </c>
+      <c r="H169" s="1">
+        <v>565562</v>
+      </c>
+      <c r="I169" s="1">
+        <v>130</v>
+      </c>
+      <c r="O169" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P169" s="1">
+        <v>271644</v>
+      </c>
+      <c r="Q169" s="1">
+        <v>32</v>
+      </c>
+      <c r="R169" s="1">
+        <v>690227</v>
+      </c>
+      <c r="S169" s="1">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="170" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A170" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B170" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F170" s="1">
+        <v>288907</v>
+      </c>
+      <c r="G170" s="1">
+        <v>128</v>
+      </c>
+      <c r="H170" s="1">
+        <v>498664</v>
+      </c>
+      <c r="I170" s="1">
+        <v>229</v>
+      </c>
+      <c r="O170" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P170" s="1">
+        <v>352816</v>
+      </c>
+      <c r="Q170" s="1">
+        <v>94</v>
+      </c>
+      <c r="R170" s="1">
+        <v>543129</v>
+      </c>
+      <c r="S170" s="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="171" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A171" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B171" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F171" s="1">
+        <v>278714</v>
+      </c>
+      <c r="G171" s="1">
+        <v>11</v>
+      </c>
+      <c r="H171" s="1">
+        <v>511467</v>
+      </c>
+      <c r="I171" s="1">
+        <v>63</v>
+      </c>
+      <c r="O171" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P171" s="1">
+        <v>317669</v>
+      </c>
+      <c r="Q171" s="1">
+        <v>14</v>
+      </c>
+      <c r="R171" s="1">
+        <v>531331</v>
+      </c>
+      <c r="S171" s="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="172" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A172" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B172" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F172" s="1">
+        <v>221210</v>
+      </c>
+      <c r="G172" s="1">
+        <v>118</v>
+      </c>
+      <c r="H172" s="1">
+        <v>678763</v>
+      </c>
+      <c r="I172" s="1">
+        <v>133</v>
+      </c>
+      <c r="O172" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P172" s="1">
+        <v>247318</v>
+      </c>
+      <c r="Q172" s="1">
+        <v>129</v>
+      </c>
+      <c r="R172" s="1">
+        <v>742142</v>
+      </c>
+      <c r="S172" s="1">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="173" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A173" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B173" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F173" s="1">
+        <v>179604</v>
+      </c>
+      <c r="G173" s="1">
+        <v>98</v>
+      </c>
+      <c r="H173" s="1">
+        <v>913108</v>
+      </c>
+      <c r="I173" s="1">
+        <v>275</v>
+      </c>
+      <c r="O173" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P173" s="1">
+        <v>212438</v>
+      </c>
+      <c r="Q173" s="1">
+        <v>99</v>
+      </c>
+      <c r="R173" s="1">
+        <v>817217</v>
+      </c>
+      <c r="S173" s="1">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="174" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A174" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B174" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F174" s="1">
+        <v>195026</v>
+      </c>
+      <c r="G174" s="1">
+        <v>52</v>
+      </c>
+      <c r="H174" s="1">
+        <v>492503</v>
+      </c>
+      <c r="I174" s="1">
+        <v>100</v>
+      </c>
+      <c r="O174" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P174" s="1">
+        <v>248058</v>
+      </c>
+      <c r="Q174" s="1">
+        <v>46</v>
+      </c>
+      <c r="R174" s="1">
+        <v>664374</v>
+      </c>
+      <c r="S174" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="175" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A175" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B175" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F175" s="1">
+        <v>240824</v>
+      </c>
+      <c r="G175" s="1">
+        <v>117</v>
+      </c>
+      <c r="H175" s="1">
+        <v>429154</v>
+      </c>
+      <c r="I175" s="1">
+        <v>134</v>
+      </c>
+      <c r="O175" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P175" s="1">
+        <v>213796</v>
+      </c>
+      <c r="Q175" s="1">
+        <v>115</v>
+      </c>
+      <c r="R175" s="1">
+        <v>620071</v>
+      </c>
+      <c r="S175" s="1">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="176" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A176" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B176" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F176" s="1">
+        <v>317437</v>
+      </c>
+      <c r="G176" s="1">
+        <v>40</v>
+      </c>
+      <c r="H176" s="1">
+        <v>512618</v>
+      </c>
+      <c r="I176" s="1">
+        <v>116</v>
+      </c>
+      <c r="O176" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P176" s="1">
+        <v>362810</v>
+      </c>
+      <c r="Q176" s="1">
+        <v>39</v>
+      </c>
+      <c r="R176" s="1">
+        <v>596906</v>
+      </c>
+      <c r="S176" s="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="177" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A177" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B177" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F177" s="1">
+        <v>234164</v>
+      </c>
+      <c r="G177" s="1">
+        <v>74</v>
+      </c>
+      <c r="H177" s="1">
+        <v>639247</v>
+      </c>
+      <c r="I177" s="1">
+        <v>60</v>
+      </c>
+      <c r="O177" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P177" s="1">
+        <v>258946</v>
+      </c>
+      <c r="Q177" s="1">
+        <v>49</v>
+      </c>
+      <c r="R177" s="1">
+        <v>976477</v>
+      </c>
+      <c r="S177" s="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="178" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A178" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B178" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F178" s="1">
+        <v>240982</v>
+      </c>
+      <c r="G178" s="1">
+        <v>88</v>
+      </c>
+      <c r="H178" s="1">
+        <v>462149</v>
+      </c>
+      <c r="I178" s="1">
+        <v>137</v>
+      </c>
+      <c r="O178" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P178" s="1">
+        <v>267589</v>
+      </c>
+      <c r="Q178" s="1">
+        <v>92</v>
+      </c>
+      <c r="R178" s="1">
+        <v>588980</v>
+      </c>
+      <c r="S178" s="1">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="179" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A179" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B179" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F179" s="1">
+        <v>253482</v>
+      </c>
+      <c r="G179" s="1">
+        <v>40</v>
+      </c>
+      <c r="H179" s="1">
+        <v>528997</v>
+      </c>
+      <c r="I179" s="1">
+        <v>80</v>
+      </c>
+      <c r="O179" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P179" s="1">
+        <v>295338</v>
+      </c>
+      <c r="Q179" s="1">
+        <v>27</v>
+      </c>
+      <c r="R179" s="1">
+        <v>597942</v>
+      </c>
+      <c r="S179" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="180" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A180" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B180" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F180" s="1">
+        <v>325545</v>
+      </c>
+      <c r="G180" s="1">
+        <v>89</v>
+      </c>
+      <c r="H180" s="1">
+        <v>531133</v>
+      </c>
+      <c r="I180" s="1">
+        <v>151</v>
+      </c>
+      <c r="O180" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P180" s="1">
+        <v>358912</v>
+      </c>
+      <c r="Q180" s="1">
+        <v>57</v>
+      </c>
+      <c r="R180" s="1">
+        <v>614084</v>
+      </c>
+      <c r="S180" s="1">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="181" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A181" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B181" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F181" s="1">
+        <v>256915</v>
+      </c>
+      <c r="G181" s="1">
+        <v>28</v>
+      </c>
+      <c r="H181" s="1">
+        <v>639566</v>
+      </c>
+      <c r="I181" s="1">
+        <v>140</v>
+      </c>
+      <c r="O181" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P181" s="1">
+        <v>285927</v>
+      </c>
+      <c r="Q181" s="1">
+        <v>12</v>
+      </c>
+      <c r="R181" s="1">
+        <v>754224</v>
+      </c>
+      <c r="S181" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="182" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A182" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B182" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F182" s="1">
+        <v>222077</v>
+      </c>
+      <c r="G182" s="1">
+        <v>46</v>
+      </c>
+      <c r="H182" s="1">
+        <v>539856</v>
+      </c>
+      <c r="I182" s="1">
+        <v>132</v>
+      </c>
+      <c r="O182" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P182" s="1">
+        <v>271397</v>
+      </c>
+      <c r="Q182" s="1">
+        <v>42</v>
+      </c>
+      <c r="R182" s="1">
+        <v>636803</v>
+      </c>
+      <c r="S182" s="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="183" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A183" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B183" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F183" s="1">
+        <v>313015</v>
+      </c>
+      <c r="G183" s="1">
+        <v>30</v>
+      </c>
+      <c r="H183" s="1">
+        <v>525334</v>
+      </c>
+      <c r="I183" s="1">
+        <v>65</v>
+      </c>
+      <c r="O183" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P183" s="1">
+        <v>348341</v>
+      </c>
+      <c r="Q183" s="1">
+        <v>17</v>
+      </c>
+      <c r="R183" s="1">
+        <v>627933</v>
+      </c>
+      <c r="S183" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="184" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A184" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B184" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F184" s="1">
+        <v>287491</v>
+      </c>
+      <c r="G184" s="1">
+        <v>44</v>
+      </c>
+      <c r="H184" s="1">
+        <v>506432</v>
+      </c>
+      <c r="I184" s="1">
+        <v>45</v>
+      </c>
+      <c r="O184" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P184" s="1">
+        <v>321208</v>
+      </c>
+      <c r="Q184" s="1">
+        <v>48</v>
+      </c>
+      <c r="R184" s="1">
+        <v>576839</v>
+      </c>
+      <c r="S184" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="185" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A185" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B185" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F185" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G185" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H185" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I185" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="O185" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P185" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q185" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R185" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="S185" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="186" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A186" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B186" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F186" s="1">
+        <v>241154</v>
+      </c>
+      <c r="G186" s="1">
+        <v>104</v>
+      </c>
+      <c r="H186" s="1">
+        <v>423178</v>
+      </c>
+      <c r="I186" s="1">
+        <v>177</v>
+      </c>
+      <c r="O186" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P186" s="1">
+        <v>267863</v>
+      </c>
+      <c r="Q186" s="1">
+        <v>67</v>
+      </c>
+      <c r="R186" s="1">
+        <v>693033</v>
+      </c>
+      <c r="S186" s="1">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="187" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A187" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B187" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F187" s="1">
+        <v>283311</v>
+      </c>
+      <c r="G187" s="1">
+        <v>34</v>
+      </c>
+      <c r="H187" s="1">
+        <v>679332</v>
+      </c>
+      <c r="I187" s="1">
+        <v>203</v>
+      </c>
+      <c r="O187" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P187" s="1">
+        <v>314144</v>
+      </c>
+      <c r="Q187" s="1">
+        <v>18</v>
+      </c>
+      <c r="R187" s="1">
+        <v>484392</v>
+      </c>
+      <c r="S187" s="1">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="188" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A188" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B188" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F188" s="1">
+        <v>229061</v>
+      </c>
+      <c r="G188" s="1">
+        <v>46</v>
+      </c>
+      <c r="H188" s="1">
+        <v>666335</v>
+      </c>
+      <c r="I188" s="1">
+        <v>162</v>
+      </c>
+      <c r="O188" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P188" s="1">
+        <v>263759</v>
+      </c>
+      <c r="Q188" s="1">
+        <v>49</v>
+      </c>
+      <c r="R188" s="1">
+        <v>752667</v>
+      </c>
+      <c r="S188" s="1">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="189" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A189" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B189" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F189" s="1">
+        <v>272501</v>
+      </c>
+      <c r="G189" s="1">
+        <v>71</v>
+      </c>
+      <c r="H189" s="1">
+        <v>562812</v>
+      </c>
+      <c r="I189" s="1">
+        <v>112</v>
+      </c>
+      <c r="O189" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P189" s="1">
+        <v>312268</v>
+      </c>
+      <c r="Q189" s="1">
+        <v>46</v>
+      </c>
+      <c r="R189" s="1">
+        <v>714141</v>
+      </c>
+      <c r="S189" s="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="190" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A190" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B190" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F190" s="1">
+        <v>133558</v>
+      </c>
+      <c r="G190" s="1">
+        <v>6</v>
+      </c>
+      <c r="H190" s="1">
+        <v>696068</v>
+      </c>
+      <c r="I190" s="1">
+        <v>54</v>
+      </c>
+      <c r="O190" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P190" s="1">
+        <v>168815</v>
+      </c>
+      <c r="Q190" s="1">
+        <v>19</v>
+      </c>
+      <c r="R190" s="1">
+        <v>772242</v>
+      </c>
+      <c r="S190" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="191" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A191" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B191" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D191" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F191" s="1">
+        <v>329988</v>
+      </c>
+      <c r="G191" s="1">
+        <v>25</v>
+      </c>
+      <c r="H191" s="1">
+        <v>640984</v>
+      </c>
+      <c r="I191" s="1">
+        <v>121</v>
+      </c>
+      <c r="O191" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P191" s="1">
+        <v>380515</v>
+      </c>
+      <c r="Q191" s="1">
+        <v>14</v>
+      </c>
+      <c r="R191" s="1">
+        <v>725380</v>
+      </c>
+      <c r="S191" s="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="192" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A192" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B192" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F192" s="1">
+        <v>266040</v>
+      </c>
+      <c r="G192" s="1">
+        <v>17</v>
+      </c>
+      <c r="H192" s="1">
+        <v>596364</v>
+      </c>
+      <c r="I192" s="1">
+        <v>72</v>
+      </c>
+      <c r="O192" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P192" s="1">
+        <v>311338</v>
+      </c>
+      <c r="Q192" s="1">
+        <v>15</v>
+      </c>
+      <c r="R192" s="1">
+        <v>711153</v>
+      </c>
+      <c r="S192" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="193" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A193" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B193" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F193" s="1">
+        <v>172760</v>
+      </c>
+      <c r="G193" s="1">
+        <v>84</v>
+      </c>
+      <c r="H193" s="1">
+        <v>697973</v>
+      </c>
+      <c r="I193" s="1">
+        <v>135</v>
+      </c>
+      <c r="O193" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P193" s="1">
+        <v>299143</v>
+      </c>
+      <c r="Q193" s="1">
+        <v>26</v>
+      </c>
+      <c r="R193" s="1">
+        <v>631124</v>
+      </c>
+      <c r="S193" s="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="194" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A194" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B194" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F194" s="1">
+        <v>86518</v>
+      </c>
+      <c r="G194" s="1">
+        <v>60</v>
+      </c>
+      <c r="H194" s="1">
+        <v>833267</v>
+      </c>
+      <c r="I194" s="1">
+        <v>282</v>
+      </c>
+      <c r="O194" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P194" s="1">
+        <v>332295</v>
+      </c>
+      <c r="Q194" s="1">
+        <v>37</v>
+      </c>
+      <c r="R194" s="1">
+        <v>746016</v>
+      </c>
+      <c r="S194" s="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="195" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A195" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B195" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F195" s="1">
+        <v>240764</v>
+      </c>
+      <c r="G195" s="1">
+        <v>108</v>
+      </c>
+      <c r="H195" s="1">
+        <v>931169</v>
+      </c>
+      <c r="I195" s="1">
+        <v>122</v>
+      </c>
+      <c r="O195" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P195" s="1">
+        <v>271518</v>
+      </c>
+      <c r="Q195" s="1">
+        <v>17</v>
+      </c>
+      <c r="R195" s="1">
+        <v>815766</v>
+      </c>
+      <c r="S195" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="196" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A196" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B196" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F196" s="1">
+        <v>295327</v>
+      </c>
+      <c r="G196" s="1">
+        <v>45</v>
+      </c>
+      <c r="H196" s="1">
+        <v>547303</v>
+      </c>
+      <c r="I196" s="1">
+        <v>136</v>
+      </c>
+      <c r="O196" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P196" s="1">
+        <v>380582</v>
+      </c>
+      <c r="Q196" s="1">
+        <v>51</v>
+      </c>
+      <c r="R196" s="1">
+        <v>576844</v>
+      </c>
+      <c r="S196" s="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="197" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A197" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B197" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F197" s="1">
+        <v>163204</v>
+      </c>
+      <c r="G197" s="1">
+        <v>42</v>
+      </c>
+      <c r="H197" s="1">
+        <v>696838</v>
+      </c>
+      <c r="I197" s="1">
+        <v>213</v>
+      </c>
+      <c r="O197" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P197" s="1">
+        <v>184413</v>
+      </c>
+      <c r="Q197" s="1">
+        <v>47</v>
+      </c>
+      <c r="R197" s="1">
+        <v>886035</v>
+      </c>
+      <c r="S197" s="1">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="198" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A198" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B198" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F198" s="1">
+        <v>332617</v>
+      </c>
+      <c r="G198" s="1">
+        <v>18</v>
+      </c>
+      <c r="H198" s="1">
+        <v>601754</v>
+      </c>
+      <c r="I198" s="1">
+        <v>97</v>
+      </c>
+      <c r="O198" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P198" s="1">
+        <v>373857</v>
+      </c>
+      <c r="Q198" s="1">
+        <v>17</v>
+      </c>
+      <c r="R198" s="1">
+        <v>689295</v>
+      </c>
+      <c r="S198" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="199" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A199" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B199" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F199" s="1">
+        <v>307097</v>
+      </c>
+      <c r="G199" s="1">
+        <v>68</v>
+      </c>
+      <c r="H199" s="1">
+        <v>562038</v>
+      </c>
+      <c r="I199" s="1">
+        <v>197</v>
+      </c>
+      <c r="O199" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P199" s="1">
+        <v>335411</v>
+      </c>
+      <c r="Q199" s="1">
+        <v>40</v>
+      </c>
+      <c r="R199" s="1">
+        <v>727754</v>
+      </c>
+      <c r="S199" s="1">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="200" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A200" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B200" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F200" s="1">
+        <v>293330</v>
+      </c>
+      <c r="G200" s="1">
+        <v>59</v>
+      </c>
+      <c r="H200" s="1">
+        <v>623542</v>
+      </c>
+      <c r="I200" s="1">
+        <v>150</v>
+      </c>
+      <c r="O200" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P200" s="1">
+        <v>330675</v>
+      </c>
+      <c r="Q200" s="1">
+        <v>44</v>
+      </c>
+      <c r="R200" s="1">
+        <v>702590</v>
+      </c>
+      <c r="S200" s="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="201" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A201" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B201" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F201" s="1">
+        <v>342394</v>
+      </c>
+      <c r="G201" s="1">
+        <v>118</v>
+      </c>
+      <c r="H201" s="1">
+        <v>541019</v>
+      </c>
+      <c r="I201" s="1">
+        <v>259</v>
+      </c>
+      <c r="O201" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P201" s="1">
+        <v>385233</v>
+      </c>
+      <c r="Q201" s="1">
+        <v>92</v>
+      </c>
+      <c r="R201" s="1">
+        <v>622151</v>
+      </c>
+      <c r="S201" s="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="202" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A202" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B202" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F202" s="1">
+        <v>358148</v>
+      </c>
+      <c r="G202" s="1">
+        <v>52</v>
+      </c>
+      <c r="H202" s="1">
+        <v>475008</v>
+      </c>
+      <c r="I202" s="1">
+        <v>126</v>
+      </c>
+      <c r="O202" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P202" s="1">
+        <v>400707</v>
+      </c>
+      <c r="Q202" s="1">
+        <v>38</v>
+      </c>
+      <c r="R202" s="1">
+        <v>562369</v>
+      </c>
+      <c r="S202" s="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="203" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A203" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B203" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O203" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="204" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A204" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B204" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="O204" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="205" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A205" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B205" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="O205" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="206" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A206" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B206" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D206" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="O206" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="207" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A207" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B207" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="O207" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="208" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A208" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B208" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="O208" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="209" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A209" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B209" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="O209" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="210" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A210" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B210" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="O210" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="211" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A211" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B211" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="O211" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="212" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A212" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B212" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="O212" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="213" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A213" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B213" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="214" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A214" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B214" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="215" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A215" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B215" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D215" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="216" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A216" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B216" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="217" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A217" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B217" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="218" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A218" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B218" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="219" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A219" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B219" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D219" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="220" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A220" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B220" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="221" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A221" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B221" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="222" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A222" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B222" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="223" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A223" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B223" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D223" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="224" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A224" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B224" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D224" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A225" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B225" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A226" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B226" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A227" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B227" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A228" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B228" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A229" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B229" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A230" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B230" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D230" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A231" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B231" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D231" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A232" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B232" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D232" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A233" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B233" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D233" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A234" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B234" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D234" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A235" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B235" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D235" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A236" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B236" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D236" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A237" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B237" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A238" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B238" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A239" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B239" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A240" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B240" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A241" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B241" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D241" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A242" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B242" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A243" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B243" s="1">
+        <v>2016</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Run 14 duplicates to embryo data
</commit_message>
<xml_diff>
--- a/Ionocyte/All embryo ionocyte data.xlsx
+++ b/Ionocyte/All embryo ionocyte data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teres\Documents\GitHub\MenidiaOA\Ionocyte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900ED4AE-1CD4-4FF6-A743-5260D91CCE23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5921D8-0AB0-40CE-93E7-C014F4AA1454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DAFCA9E7-78AB-4FDC-8B4B-32C2729B4956}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1304" uniqueCount="274">
   <si>
     <t>Experiment</t>
   </si>
@@ -772,9 +772,6 @@
     <t>2016-514</t>
   </si>
   <si>
-    <t>2016-515</t>
-  </si>
-  <si>
     <t>2016-516</t>
   </si>
   <si>
@@ -805,9 +802,6 @@
     <t>2016-525</t>
   </si>
   <si>
-    <t>2016-526</t>
-  </si>
-  <si>
     <t>2016-527</t>
   </si>
   <si>
@@ -854,9 +848,6 @@
   </si>
   <si>
     <t>2016-542</t>
-  </si>
-  <si>
-    <t>2016-543</t>
   </si>
   <si>
     <t>2016-544</t>
@@ -1263,11 +1254,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F1C880-24DC-4CF8-8C86-70B462FC0B54}">
-  <dimension ref="A1:X243"/>
+  <dimension ref="A1:X239"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A195" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D205" sqref="D205"/>
+      <pane ySplit="1" topLeftCell="A217" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P236" sqref="P236:S236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10213,6 +10204,18 @@
       <c r="O203" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="P203" s="1">
+        <v>391910</v>
+      </c>
+      <c r="Q203" s="1">
+        <v>30</v>
+      </c>
+      <c r="R203" s="1">
+        <v>619260</v>
+      </c>
+      <c r="S203" s="1">
+        <v>73</v>
+      </c>
     </row>
     <row r="204" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
@@ -10227,8 +10230,23 @@
       <c r="D204" s="1" t="s">
         <v>238</v>
       </c>
+      <c r="E204" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="O204" s="1" t="s">
         <v>67</v>
+      </c>
+      <c r="P204" s="1">
+        <v>365626</v>
+      </c>
+      <c r="Q204" s="1">
+        <v>116</v>
+      </c>
+      <c r="R204" s="1">
+        <v>703874</v>
+      </c>
+      <c r="S204" s="1">
+        <v>177</v>
       </c>
     </row>
     <row r="205" spans="1:19" x14ac:dyDescent="0.3">
@@ -10244,8 +10262,23 @@
       <c r="D205" s="1" t="s">
         <v>239</v>
       </c>
+      <c r="E205" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="O205" s="1" t="s">
         <v>66</v>
+      </c>
+      <c r="P205" s="1">
+        <v>143401</v>
+      </c>
+      <c r="Q205" s="1">
+        <v>46</v>
+      </c>
+      <c r="R205" s="1">
+        <v>694887</v>
+      </c>
+      <c r="S205" s="1">
+        <v>115</v>
       </c>
     </row>
     <row r="206" spans="1:19" x14ac:dyDescent="0.3">
@@ -10261,8 +10294,23 @@
       <c r="D206" s="1" t="s">
         <v>240</v>
       </c>
+      <c r="E206" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="O206" s="1" t="s">
         <v>66</v>
+      </c>
+      <c r="P206" s="1">
+        <v>204743</v>
+      </c>
+      <c r="Q206" s="1">
+        <v>4</v>
+      </c>
+      <c r="R206" s="1">
+        <v>728783</v>
+      </c>
+      <c r="S206" s="1">
+        <v>88</v>
       </c>
     </row>
     <row r="207" spans="1:19" x14ac:dyDescent="0.3">
@@ -10278,8 +10326,23 @@
       <c r="D207" s="1" t="s">
         <v>241</v>
       </c>
+      <c r="E207" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="O207" s="1" t="s">
         <v>66</v>
+      </c>
+      <c r="P207" s="1">
+        <v>383088</v>
+      </c>
+      <c r="Q207" s="1">
+        <v>45</v>
+      </c>
+      <c r="R207" s="1">
+        <v>494130</v>
+      </c>
+      <c r="S207" s="1">
+        <v>112</v>
       </c>
     </row>
     <row r="208" spans="1:19" x14ac:dyDescent="0.3">
@@ -10295,11 +10358,26 @@
       <c r="D208" s="1" t="s">
         <v>242</v>
       </c>
+      <c r="E208" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="O208" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="209" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P208" s="1">
+        <v>423439</v>
+      </c>
+      <c r="Q208" s="1">
+        <v>70</v>
+      </c>
+      <c r="R208" s="1">
+        <v>798774</v>
+      </c>
+      <c r="S208" s="1">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="209" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
         <v>154</v>
       </c>
@@ -10312,11 +10390,26 @@
       <c r="D209" s="1" t="s">
         <v>243</v>
       </c>
+      <c r="E209" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="O209" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="210" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P209" s="1">
+        <v>238149</v>
+      </c>
+      <c r="Q209" s="1">
+        <v>59</v>
+      </c>
+      <c r="R209" s="1">
+        <v>920528</v>
+      </c>
+      <c r="S209" s="1">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="210" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>154</v>
       </c>
@@ -10329,11 +10422,26 @@
       <c r="D210" s="1" t="s">
         <v>244</v>
       </c>
+      <c r="E210" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="O210" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="211" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P210" s="1">
+        <v>267838</v>
+      </c>
+      <c r="Q210" s="1">
+        <v>10</v>
+      </c>
+      <c r="R210" s="1">
+        <v>583965</v>
+      </c>
+      <c r="S210" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="211" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>154</v>
       </c>
@@ -10346,11 +10454,26 @@
       <c r="D211" s="1" t="s">
         <v>245</v>
       </c>
+      <c r="E211" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="O211" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="212" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P211" s="1">
+        <v>193811</v>
+      </c>
+      <c r="Q211" s="1">
+        <v>87</v>
+      </c>
+      <c r="R211" s="1">
+        <v>882426</v>
+      </c>
+      <c r="S211" s="1">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="212" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>154</v>
       </c>
@@ -10363,11 +10486,26 @@
       <c r="D212" s="1" t="s">
         <v>246</v>
       </c>
+      <c r="E212" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="O212" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="213" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P212" s="1">
+        <v>196677</v>
+      </c>
+      <c r="Q212" s="1">
+        <v>91</v>
+      </c>
+      <c r="R212" s="1">
+        <v>694499</v>
+      </c>
+      <c r="S212" s="1">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="213" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
         <v>154</v>
       </c>
@@ -10380,8 +10518,26 @@
       <c r="D213" s="1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="214" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E213" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O213" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P213" s="1">
+        <v>217632</v>
+      </c>
+      <c r="Q213" s="1">
+        <v>11</v>
+      </c>
+      <c r="R213" s="1">
+        <v>471379</v>
+      </c>
+      <c r="S213" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="214" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
         <v>154</v>
       </c>
@@ -10394,8 +10550,26 @@
       <c r="D214" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="215" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E214" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O214" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P214" s="1">
+        <v>176608</v>
+      </c>
+      <c r="Q214" s="1">
+        <v>28</v>
+      </c>
+      <c r="R214" s="1">
+        <v>734244</v>
+      </c>
+      <c r="S214" s="1">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="215" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
         <v>154</v>
       </c>
@@ -10408,8 +10582,26 @@
       <c r="D215" s="1" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="216" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E215" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O215" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P215" s="1">
+        <v>281103</v>
+      </c>
+      <c r="Q215" s="1">
+        <v>32</v>
+      </c>
+      <c r="R215" s="1">
+        <v>657432</v>
+      </c>
+      <c r="S215" s="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="216" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
         <v>154</v>
       </c>
@@ -10422,8 +10614,26 @@
       <c r="D216" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E216" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O216" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P216" s="1">
+        <v>299230</v>
+      </c>
+      <c r="Q216" s="1">
+        <v>29</v>
+      </c>
+      <c r="R216" s="1">
+        <v>607408</v>
+      </c>
+      <c r="S216" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="217" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
         <v>154</v>
       </c>
@@ -10436,8 +10646,26 @@
       <c r="D217" s="1" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="218" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E217" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O217" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P217" s="1">
+        <v>160772</v>
+      </c>
+      <c r="Q217" s="1">
+        <v>82</v>
+      </c>
+      <c r="R217" s="1">
+        <v>807003</v>
+      </c>
+      <c r="S217" s="1">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="218" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
         <v>154</v>
       </c>
@@ -10450,8 +10678,26 @@
       <c r="D218" s="1" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="219" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E218" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O218" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P218" s="1">
+        <v>204096</v>
+      </c>
+      <c r="Q218" s="1">
+        <v>2</v>
+      </c>
+      <c r="R218" s="1">
+        <v>564416</v>
+      </c>
+      <c r="S218" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="219" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
         <v>154</v>
       </c>
@@ -10464,8 +10710,26 @@
       <c r="D219" s="1" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="220" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E219" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O219" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P219" s="1">
+        <v>268339</v>
+      </c>
+      <c r="Q219" s="1">
+        <v>24</v>
+      </c>
+      <c r="R219" s="1">
+        <v>757620</v>
+      </c>
+      <c r="S219" s="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="220" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
         <v>154</v>
       </c>
@@ -10478,8 +10742,26 @@
       <c r="D220" s="1" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="221" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E220" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O220" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P220" s="1">
+        <v>201472</v>
+      </c>
+      <c r="Q220" s="1">
+        <v>30</v>
+      </c>
+      <c r="R220" s="1">
+        <v>651114</v>
+      </c>
+      <c r="S220" s="1">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="221" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
         <v>154</v>
       </c>
@@ -10492,8 +10774,26 @@
       <c r="D221" s="1" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="222" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E221" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O221" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P221" s="1">
+        <v>261122</v>
+      </c>
+      <c r="Q221" s="1">
+        <v>97</v>
+      </c>
+      <c r="R221" s="1">
+        <v>648052</v>
+      </c>
+      <c r="S221" s="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="222" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>154</v>
       </c>
@@ -10506,8 +10806,26 @@
       <c r="D222" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="223" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E222" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O222" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P222" s="1">
+        <v>306371</v>
+      </c>
+      <c r="Q222" s="1">
+        <v>54</v>
+      </c>
+      <c r="R222" s="1">
+        <v>592105</v>
+      </c>
+      <c r="S222" s="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="223" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
         <v>154</v>
       </c>
@@ -10520,8 +10838,26 @@
       <c r="D223" s="1" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="224" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E223" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O223" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P223" s="1">
+        <v>232313</v>
+      </c>
+      <c r="Q223" s="1">
+        <v>79</v>
+      </c>
+      <c r="R223" s="1">
+        <v>639412</v>
+      </c>
+      <c r="S223" s="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="224" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
         <v>154</v>
       </c>
@@ -10534,8 +10870,26 @@
       <c r="D224" s="1" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E224" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O224" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P224" s="1">
+        <v>250927</v>
+      </c>
+      <c r="Q224" s="1">
+        <v>92</v>
+      </c>
+      <c r="R224" s="1">
+        <v>749992</v>
+      </c>
+      <c r="S224" s="1">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="225" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>154</v>
       </c>
@@ -10548,8 +10902,26 @@
       <c r="D225" s="1" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E225" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O225" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P225" s="1">
+        <v>245549</v>
+      </c>
+      <c r="Q225" s="1">
+        <v>34</v>
+      </c>
+      <c r="R225" s="1">
+        <v>518916</v>
+      </c>
+      <c r="S225" s="1">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="226" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>154</v>
       </c>
@@ -10562,8 +10934,14 @@
       <c r="D226" s="1" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E226" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="O226" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="227" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
         <v>154</v>
       </c>
@@ -10576,8 +10954,26 @@
       <c r="D227" s="1" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E227" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O227" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P227" s="1">
+        <v>393303</v>
+      </c>
+      <c r="Q227" s="1">
+        <v>143</v>
+      </c>
+      <c r="R227" s="1">
+        <v>520531</v>
+      </c>
+      <c r="S227" s="1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="228" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
         <v>154</v>
       </c>
@@ -10590,8 +10986,26 @@
       <c r="D228" s="1" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E228" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O228" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P228" s="1">
+        <v>384612</v>
+      </c>
+      <c r="Q228" s="1">
+        <v>42</v>
+      </c>
+      <c r="R228" s="1">
+        <v>752214</v>
+      </c>
+      <c r="S228" s="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="229" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
         <v>154</v>
       </c>
@@ -10604,8 +11018,26 @@
       <c r="D229" s="1" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E229" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O229" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P229" s="1">
+        <v>117958</v>
+      </c>
+      <c r="Q229" s="1">
+        <v>44</v>
+      </c>
+      <c r="R229" s="1">
+        <v>735869</v>
+      </c>
+      <c r="S229" s="1">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="230" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
         <v>154</v>
       </c>
@@ -10618,8 +11050,26 @@
       <c r="D230" s="1" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E230" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O230" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P230" s="1">
+        <v>238393</v>
+      </c>
+      <c r="Q230" s="1">
+        <v>47</v>
+      </c>
+      <c r="R230" s="1">
+        <v>649994</v>
+      </c>
+      <c r="S230" s="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="231" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
         <v>154</v>
       </c>
@@ -10632,8 +11082,26 @@
       <c r="D231" s="1" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E231" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O231" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P231" s="1">
+        <v>234323</v>
+      </c>
+      <c r="Q231" s="1">
+        <v>30</v>
+      </c>
+      <c r="R231" s="1">
+        <v>689145</v>
+      </c>
+      <c r="S231" s="1">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="232" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
         <v>154</v>
       </c>
@@ -10646,8 +11114,14 @@
       <c r="D232" s="1" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E232" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="O232" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="233" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
         <v>154</v>
       </c>
@@ -10660,8 +11134,26 @@
       <c r="D233" s="1" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E233" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O233" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P233" s="1">
+        <v>183664</v>
+      </c>
+      <c r="Q233" s="1">
+        <v>47</v>
+      </c>
+      <c r="R233" s="1">
+        <v>749586</v>
+      </c>
+      <c r="S233" s="1">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="234" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>154</v>
       </c>
@@ -10674,8 +11166,26 @@
       <c r="D234" s="1" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E234" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O234" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P234" s="1">
+        <v>185237</v>
+      </c>
+      <c r="Q234" s="1">
+        <v>45</v>
+      </c>
+      <c r="R234" s="1">
+        <v>654479</v>
+      </c>
+      <c r="S234" s="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="235" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
         <v>154</v>
       </c>
@@ -10688,8 +11198,26 @@
       <c r="D235" s="1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E235" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O235" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P235" s="1">
+        <v>224851</v>
+      </c>
+      <c r="Q235" s="1">
+        <v>70</v>
+      </c>
+      <c r="R235" s="1">
+        <v>639664</v>
+      </c>
+      <c r="S235" s="1">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="236" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
         <v>154</v>
       </c>
@@ -10702,8 +11230,26 @@
       <c r="D236" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E236" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O236" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P236" s="1">
+        <v>273473</v>
+      </c>
+      <c r="Q236" s="1">
+        <v>79</v>
+      </c>
+      <c r="R236" s="1">
+        <v>584624</v>
+      </c>
+      <c r="S236" s="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="237" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
         <v>154</v>
       </c>
@@ -10716,8 +11262,26 @@
       <c r="D237" s="1" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E237" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O237" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P237" s="1">
+        <v>257052</v>
+      </c>
+      <c r="Q237" s="1">
+        <v>25</v>
+      </c>
+      <c r="R237" s="1">
+        <v>671998</v>
+      </c>
+      <c r="S237" s="1">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="238" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
         <v>154</v>
       </c>
@@ -10730,8 +11294,26 @@
       <c r="D238" s="1" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E238" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O238" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P238" s="1">
+        <v>283354</v>
+      </c>
+      <c r="Q238" s="1">
+        <v>72</v>
+      </c>
+      <c r="R238" s="1">
+        <v>609310</v>
+      </c>
+      <c r="S238" s="1">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="239" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
         <v>154</v>
       </c>
@@ -10744,58 +11326,23 @@
       <c r="D239" s="1" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A240" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B240" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C240" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D240" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A241" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B241" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C241" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D241" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A242" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B242" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C242" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D242" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A243" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B243" s="1">
-        <v>2016</v>
-      </c>
-      <c r="C243" s="1" t="s">
-        <v>236</v>
+      <c r="E239" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O239" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P239" s="1">
+        <v>231044</v>
+      </c>
+      <c r="Q239" s="1">
+        <v>61</v>
+      </c>
+      <c r="R239" s="1">
+        <v>839375</v>
+      </c>
+      <c r="S239" s="1">
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished entering 2016 data embryos
</commit_message>
<xml_diff>
--- a/Ionocyte/All embryo ionocyte data.xlsx
+++ b/Ionocyte/All embryo ionocyte data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teres\Documents\GitHub\MenidiaOA\Ionocyte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA38DA6-1CC7-4FFE-B420-6CFB10D6D50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108FADDF-1066-440A-92D3-6C48E00B2507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DAFCA9E7-78AB-4FDC-8B4B-32C2729B4956}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="INFO" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1304" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="274">
   <si>
     <t>Experiment</t>
   </si>
@@ -1258,8 +1257,8 @@
   <dimension ref="A1:X239"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A217" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P236" sqref="P236:S236"/>
+      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L233" sqref="L233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10202,6 +10201,18 @@
       <c r="E203" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="F203" s="1">
+        <v>353562</v>
+      </c>
+      <c r="G203" s="1">
+        <v>48</v>
+      </c>
+      <c r="H203" s="1">
+        <v>523597</v>
+      </c>
+      <c r="I203" s="1">
+        <v>199</v>
+      </c>
       <c r="O203" s="1" t="s">
         <v>67</v>
       </c>
@@ -10234,6 +10245,18 @@
       <c r="E204" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="F204" s="1">
+        <v>313698</v>
+      </c>
+      <c r="G204" s="1">
+        <v>150</v>
+      </c>
+      <c r="H204" s="1">
+        <v>629227</v>
+      </c>
+      <c r="I204" s="1">
+        <v>287</v>
+      </c>
       <c r="O204" s="1" t="s">
         <v>67</v>
       </c>
@@ -10266,6 +10289,18 @@
       <c r="E205" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F205" s="1">
+        <v>120790</v>
+      </c>
+      <c r="G205" s="1">
+        <v>55</v>
+      </c>
+      <c r="H205" s="1">
+        <v>656212</v>
+      </c>
+      <c r="I205" s="1">
+        <v>219</v>
+      </c>
       <c r="O205" s="1" t="s">
         <v>66</v>
       </c>
@@ -10296,7 +10331,19 @@
         <v>240</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
+      </c>
+      <c r="F206" s="1">
+        <v>148627</v>
+      </c>
+      <c r="G206" s="1">
+        <v>50</v>
+      </c>
+      <c r="H206" s="1">
+        <v>755045</v>
+      </c>
+      <c r="I206" s="1">
+        <v>305</v>
       </c>
       <c r="O206" s="1" t="s">
         <v>66</v>
@@ -10330,6 +10377,18 @@
       <c r="E207" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F207" s="1">
+        <v>306212</v>
+      </c>
+      <c r="G207" s="1">
+        <v>83</v>
+      </c>
+      <c r="H207" s="1">
+        <v>451840</v>
+      </c>
+      <c r="I207" s="1">
+        <v>184</v>
+      </c>
       <c r="O207" s="1" t="s">
         <v>66</v>
       </c>
@@ -10362,6 +10421,18 @@
       <c r="E208" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="F208" s="1">
+        <v>394277</v>
+      </c>
+      <c r="G208" s="1">
+        <v>90</v>
+      </c>
+      <c r="H208" s="1">
+        <v>652741</v>
+      </c>
+      <c r="I208" s="1">
+        <v>301</v>
+      </c>
       <c r="O208" s="1" t="s">
         <v>67</v>
       </c>
@@ -10394,6 +10465,18 @@
       <c r="E209" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="F209" s="1">
+        <v>214232</v>
+      </c>
+      <c r="G209" s="1">
+        <v>74</v>
+      </c>
+      <c r="H209" s="1">
+        <v>10224290</v>
+      </c>
+      <c r="I209" s="1">
+        <v>335</v>
+      </c>
       <c r="O209" s="1" t="s">
         <v>67</v>
       </c>
@@ -10426,6 +10509,18 @@
       <c r="E210" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="F210" s="1">
+        <v>259206</v>
+      </c>
+      <c r="G210" s="1">
+        <v>44</v>
+      </c>
+      <c r="H210" s="1">
+        <v>534428</v>
+      </c>
+      <c r="I210" s="1">
+        <v>119</v>
+      </c>
       <c r="O210" s="1" t="s">
         <v>67</v>
       </c>
@@ -10458,6 +10553,18 @@
       <c r="E211" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="F211" s="1">
+        <v>176261</v>
+      </c>
+      <c r="G211" s="1">
+        <v>137</v>
+      </c>
+      <c r="H211" s="1">
+        <v>756448</v>
+      </c>
+      <c r="I211" s="1">
+        <v>325</v>
+      </c>
       <c r="O211" s="1" t="s">
         <v>67</v>
       </c>
@@ -10490,6 +10597,18 @@
       <c r="E212" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F212" s="1">
+        <v>184731</v>
+      </c>
+      <c r="G212" s="1">
+        <v>150</v>
+      </c>
+      <c r="H212" s="1">
+        <v>495103</v>
+      </c>
+      <c r="I212" s="1">
+        <v>309</v>
+      </c>
       <c r="O212" s="1" t="s">
         <v>66</v>
       </c>
@@ -10522,6 +10641,18 @@
       <c r="E213" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="F213" s="1">
+        <v>183509</v>
+      </c>
+      <c r="G213" s="1">
+        <v>35</v>
+      </c>
+      <c r="H213" s="1">
+        <v>331943</v>
+      </c>
+      <c r="I213" s="1">
+        <v>14</v>
+      </c>
       <c r="O213" s="1" t="s">
         <v>67</v>
       </c>
@@ -10554,6 +10685,18 @@
       <c r="E214" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F214" s="1">
+        <v>139952</v>
+      </c>
+      <c r="G214" s="1">
+        <v>49</v>
+      </c>
+      <c r="H214" s="1">
+        <v>593964</v>
+      </c>
+      <c r="I214" s="1">
+        <v>311</v>
+      </c>
       <c r="O214" s="1" t="s">
         <v>66</v>
       </c>
@@ -10584,7 +10727,19 @@
         <v>249</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
+      </c>
+      <c r="F215" s="1">
+        <v>189762</v>
+      </c>
+      <c r="G215" s="1">
+        <v>64</v>
+      </c>
+      <c r="H215" s="1">
+        <v>606373</v>
+      </c>
+      <c r="I215" s="1">
+        <v>197</v>
       </c>
       <c r="O215" s="1" t="s">
         <v>66</v>
@@ -10618,6 +10773,18 @@
       <c r="E216" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="F216" s="1">
+        <v>273636</v>
+      </c>
+      <c r="G216" s="1">
+        <v>64</v>
+      </c>
+      <c r="H216" s="1">
+        <v>460342</v>
+      </c>
+      <c r="I216" s="1">
+        <v>151</v>
+      </c>
       <c r="O216" s="1" t="s">
         <v>67</v>
       </c>
@@ -10650,6 +10817,18 @@
       <c r="E217" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="F217" s="1">
+        <v>144104</v>
+      </c>
+      <c r="G217" s="1">
+        <v>110</v>
+      </c>
+      <c r="H217" s="1">
+        <v>616080</v>
+      </c>
+      <c r="I217" s="1">
+        <v>250</v>
+      </c>
       <c r="O217" s="1" t="s">
         <v>67</v>
       </c>
@@ -10682,6 +10861,18 @@
       <c r="E218" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F218" s="1">
+        <v>139398</v>
+      </c>
+      <c r="G218" s="1">
+        <v>29</v>
+      </c>
+      <c r="H218" s="1">
+        <v>549610</v>
+      </c>
+      <c r="I218" s="1">
+        <v>176</v>
+      </c>
       <c r="O218" s="1" t="s">
         <v>66</v>
       </c>
@@ -10712,7 +10903,19 @@
         <v>253</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="F219" s="1">
+        <v>264966</v>
+      </c>
+      <c r="G219" s="1">
+        <v>56</v>
+      </c>
+      <c r="H219" s="1">
+        <v>618484</v>
+      </c>
+      <c r="I219" s="1">
+        <v>173</v>
       </c>
       <c r="O219" s="1" t="s">
         <v>67</v>
@@ -10744,7 +10947,19 @@
         <v>254</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="F220" s="1">
+        <v>167438</v>
+      </c>
+      <c r="G220" s="1">
+        <v>128</v>
+      </c>
+      <c r="H220" s="1">
+        <v>611786</v>
+      </c>
+      <c r="I220" s="1">
+        <v>263</v>
       </c>
       <c r="O220" s="1" t="s">
         <v>67</v>
@@ -10776,7 +10991,19 @@
         <v>255</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
+      </c>
+      <c r="F221" s="1">
+        <v>166458</v>
+      </c>
+      <c r="G221" s="1">
+        <v>108</v>
+      </c>
+      <c r="H221" s="1">
+        <v>788662</v>
+      </c>
+      <c r="I221" s="1">
+        <v>229</v>
       </c>
       <c r="O221" s="1" t="s">
         <v>66</v>
@@ -10810,6 +11037,18 @@
       <c r="E222" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F222" s="1">
+        <v>286996</v>
+      </c>
+      <c r="G222" s="1">
+        <v>84</v>
+      </c>
+      <c r="H222" s="1">
+        <v>496598</v>
+      </c>
+      <c r="I222" s="1">
+        <v>116</v>
+      </c>
       <c r="O222" s="1" t="s">
         <v>66</v>
       </c>
@@ -10840,7 +11079,19 @@
         <v>257</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="F223" s="1">
+        <v>152683</v>
+      </c>
+      <c r="G223" s="1">
+        <v>88</v>
+      </c>
+      <c r="H223" s="1">
+        <v>619601</v>
+      </c>
+      <c r="I223" s="1">
+        <v>240</v>
       </c>
       <c r="O223" s="1" t="s">
         <v>67</v>
@@ -10874,6 +11125,18 @@
       <c r="E224" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F224" s="1">
+        <v>226233</v>
+      </c>
+      <c r="G224" s="1">
+        <v>104</v>
+      </c>
+      <c r="H224" s="1">
+        <v>603649</v>
+      </c>
+      <c r="I224" s="1">
+        <v>304</v>
+      </c>
       <c r="O224" s="1" t="s">
         <v>66</v>
       </c>
@@ -10906,6 +11169,18 @@
       <c r="E225" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F225" s="1">
+        <v>141389</v>
+      </c>
+      <c r="G225" s="1">
+        <v>42</v>
+      </c>
+      <c r="H225" s="1">
+        <v>705803</v>
+      </c>
+      <c r="I225" s="1">
+        <v>247</v>
+      </c>
       <c r="O225" s="1" t="s">
         <v>66</v>
       </c>
@@ -10938,7 +11213,31 @@
       <c r="E226" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="F226" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G226" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H226" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I226" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="O226" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P226" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q226" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R226" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="S226" s="1" t="s">
         <v>109</v>
       </c>
     </row>
@@ -10958,6 +11257,18 @@
       <c r="E227" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F227" s="1">
+        <v>267069</v>
+      </c>
+      <c r="G227" s="1">
+        <v>128</v>
+      </c>
+      <c r="H227" s="1">
+        <v>505954</v>
+      </c>
+      <c r="I227" s="1">
+        <v>229</v>
+      </c>
       <c r="O227" s="1" t="s">
         <v>66</v>
       </c>
@@ -10988,7 +11299,19 @@
         <v>262</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="F228" s="1">
+        <v>223385</v>
+      </c>
+      <c r="G228" s="1">
+        <v>63</v>
+      </c>
+      <c r="H228" s="1">
+        <v>819133</v>
+      </c>
+      <c r="I228" s="1">
+        <v>161</v>
       </c>
       <c r="O228" s="1" t="s">
         <v>67</v>
@@ -11022,6 +11345,18 @@
       <c r="E229" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F229" s="1">
+        <v>101321</v>
+      </c>
+      <c r="G229" s="1">
+        <v>61</v>
+      </c>
+      <c r="H229" s="1">
+        <v>595781</v>
+      </c>
+      <c r="I229" s="1">
+        <v>341</v>
+      </c>
       <c r="O229" s="1" t="s">
         <v>66</v>
       </c>
@@ -11054,6 +11389,18 @@
       <c r="E230" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F230" s="1">
+        <v>187463</v>
+      </c>
+      <c r="G230" s="1">
+        <v>91</v>
+      </c>
+      <c r="H230" s="1">
+        <v>576577</v>
+      </c>
+      <c r="I230" s="1">
+        <v>144</v>
+      </c>
       <c r="O230" s="1" t="s">
         <v>66</v>
       </c>
@@ -11086,6 +11433,18 @@
       <c r="E231" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F231" s="1">
+        <v>226767</v>
+      </c>
+      <c r="G231" s="1">
+        <v>63</v>
+      </c>
+      <c r="H231" s="1">
+        <v>556146</v>
+      </c>
+      <c r="I231" s="1">
+        <v>219</v>
+      </c>
       <c r="O231" s="1" t="s">
         <v>66</v>
       </c>
@@ -11118,7 +11477,31 @@
       <c r="E232" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="F232" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G232" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H232" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I232" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="O232" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P232" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q232" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R232" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="S232" s="1" t="s">
         <v>109</v>
       </c>
     </row>
@@ -11136,7 +11519,19 @@
         <v>267</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="F233" s="1">
+        <v>233934</v>
+      </c>
+      <c r="G233" s="1">
+        <v>33</v>
+      </c>
+      <c r="H233" s="1">
+        <v>439524</v>
+      </c>
+      <c r="I233" s="1">
+        <v>133</v>
       </c>
       <c r="O233" s="1" t="s">
         <v>67</v>
@@ -11170,6 +11565,18 @@
       <c r="E234" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F234" s="1">
+        <v>170029</v>
+      </c>
+      <c r="G234" s="1">
+        <v>81</v>
+      </c>
+      <c r="H234" s="1">
+        <v>500161</v>
+      </c>
+      <c r="I234" s="1">
+        <v>289</v>
+      </c>
       <c r="O234" s="1" t="s">
         <v>66</v>
       </c>
@@ -11202,6 +11609,18 @@
       <c r="E235" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F235" s="1">
+        <v>167129</v>
+      </c>
+      <c r="G235" s="1">
+        <v>80</v>
+      </c>
+      <c r="H235" s="1">
+        <v>543545</v>
+      </c>
+      <c r="I235" s="1">
+        <v>305</v>
+      </c>
       <c r="O235" s="1" t="s">
         <v>66</v>
       </c>
@@ -11232,7 +11651,19 @@
         <v>270</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="F236" s="1">
+        <v>132168</v>
+      </c>
+      <c r="G236" s="1">
+        <v>110</v>
+      </c>
+      <c r="H236" s="1">
+        <v>614676</v>
+      </c>
+      <c r="I236" s="1">
+        <v>359</v>
       </c>
       <c r="O236" s="1" t="s">
         <v>67</v>
@@ -11264,7 +11695,19 @@
         <v>271</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
+      </c>
+      <c r="F237" s="1">
+        <v>162133</v>
+      </c>
+      <c r="G237" s="1">
+        <v>100</v>
+      </c>
+      <c r="H237" s="1">
+        <v>739948</v>
+      </c>
+      <c r="I237" s="1">
+        <v>392</v>
       </c>
       <c r="O237" s="1" t="s">
         <v>66</v>
@@ -11298,6 +11741,18 @@
       <c r="E238" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="F238" s="1">
+        <v>306476</v>
+      </c>
+      <c r="G238" s="1">
+        <v>143</v>
+      </c>
+      <c r="H238" s="1">
+        <v>441301</v>
+      </c>
+      <c r="I238" s="1">
+        <v>228</v>
+      </c>
       <c r="O238" s="1" t="s">
         <v>66</v>
       </c>
@@ -11329,6 +11784,18 @@
       </c>
       <c r="E239" s="1" t="s">
         <v>66</v>
+      </c>
+      <c r="F239" s="1">
+        <v>322644</v>
+      </c>
+      <c r="G239" s="1">
+        <v>154</v>
+      </c>
+      <c r="H239" s="1">
+        <v>523646</v>
+      </c>
+      <c r="I239" s="1">
+        <v>258</v>
       </c>
       <c r="O239" s="1" t="s">
         <v>66</v>

</xml_diff>